<commit_message>
Added the 3 attributes of interest to merged data file: 'Country', 'Number of People Living with HIV', 'Descrimination Percent'
</commit_message>
<xml_diff>
--- a/GlobalHIVMerged.xlsx
+++ b/GlobalHIVMerged.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14600" tabRatio="500"/>
+    <workbookView xWindow="1640" yWindow="4940" windowWidth="25600" windowHeight="14580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,20 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Number of People Living with HIV</t>
+  </si>
+  <si>
+    <t>Descrimination Percent</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -336,14 +350,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Copy and pasted Country attribute records (1 to 1) from HIVDescrimination.xls to GlobalHIVMerged.xlsx because there are fewer countries in HIVDescrimination.xls than HIVPopulation.xls so it will be the limiting set.
</commit_message>
<xml_diff>
--- a/GlobalHIVMerged.xlsx
+++ b/GlobalHIVMerged.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1640" yWindow="4940" windowWidth="25600" windowHeight="14580" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="25600" windowHeight="14580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>Country</t>
   </si>
@@ -36,6 +36,183 @@
   </si>
   <si>
     <t>Descrimination Percent</t>
+  </si>
+  <si>
+    <t>Afghanistan</t>
+  </si>
+  <si>
+    <t>Albania</t>
+  </si>
+  <si>
+    <t>Angola</t>
+  </si>
+  <si>
+    <t>Armenia</t>
+  </si>
+  <si>
+    <t>Belize</t>
+  </si>
+  <si>
+    <t>Benin</t>
+  </si>
+  <si>
+    <t>Bolivia (Plurinational State of)</t>
+  </si>
+  <si>
+    <t>Bosnia and Herzegovina</t>
+  </si>
+  <si>
+    <t>Botswana</t>
+  </si>
+  <si>
+    <t>Burkina Faso</t>
+  </si>
+  <si>
+    <t>Burundi</t>
+  </si>
+  <si>
+    <t>Cambodia</t>
+  </si>
+  <si>
+    <t>Cameroon</t>
+  </si>
+  <si>
+    <t>Central African Republic</t>
+  </si>
+  <si>
+    <t>Comoros</t>
+  </si>
+  <si>
+    <t>Congo</t>
+  </si>
+  <si>
+    <t>Cuba</t>
+  </si>
+  <si>
+    <t>Côte d'Ivoire</t>
+  </si>
+  <si>
+    <t>Democratic Republic of the Congo</t>
+  </si>
+  <si>
+    <t>Dominican Republic</t>
+  </si>
+  <si>
+    <t>Ethiopia</t>
+  </si>
+  <si>
+    <t>Gabon</t>
+  </si>
+  <si>
+    <t>Gambia</t>
+  </si>
+  <si>
+    <t>Ghana</t>
+  </si>
+  <si>
+    <t>Guatemala</t>
+  </si>
+  <si>
+    <t>Guinea</t>
+  </si>
+  <si>
+    <t>Haiti</t>
+  </si>
+  <si>
+    <t>Honduras</t>
+  </si>
+  <si>
+    <t>Indonesia</t>
+  </si>
+  <si>
+    <t>Jamaica</t>
+  </si>
+  <si>
+    <t>Kazakhstan</t>
+  </si>
+  <si>
+    <t>Kenya</t>
+  </si>
+  <si>
+    <t>Kyrgyzstan</t>
+  </si>
+  <si>
+    <t>Lao People's Democratic Republic</t>
+  </si>
+  <si>
+    <t>Lesotho</t>
+  </si>
+  <si>
+    <t>Liberia</t>
+  </si>
+  <si>
+    <t>Malawi</t>
+  </si>
+  <si>
+    <t>Mali</t>
+  </si>
+  <si>
+    <t>Mongolia</t>
+  </si>
+  <si>
+    <t>Montenegro</t>
+  </si>
+  <si>
+    <t>Mozambique</t>
+  </si>
+  <si>
+    <t>Namibia</t>
+  </si>
+  <si>
+    <t>Nepal</t>
+  </si>
+  <si>
+    <t>Niger</t>
+  </si>
+  <si>
+    <t>Nigeria</t>
+  </si>
+  <si>
+    <t>Pakistan</t>
+  </si>
+  <si>
+    <t>Republic of Moldova</t>
+  </si>
+  <si>
+    <t>Rwanda</t>
+  </si>
+  <si>
+    <t>Saint Vincent and the Grenadines</t>
+  </si>
+  <si>
+    <t>Senegal</t>
+  </si>
+  <si>
+    <t>Sierra Leone</t>
+  </si>
+  <si>
+    <t>Swaziland</t>
+  </si>
+  <si>
+    <t>Timor-Leste</t>
+  </si>
+  <si>
+    <t>Togo</t>
+  </si>
+  <si>
+    <t>Uganda</t>
+  </si>
+  <si>
+    <t>Ukraine</t>
+  </si>
+  <si>
+    <t>United Republic of Tanzania</t>
+  </si>
+  <si>
+    <t>Zambia</t>
+  </si>
+  <si>
+    <t>Zimbabwe</t>
   </si>
 </sst>
 </file>
@@ -350,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -369,6 +546,301 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Copy and pasted (1 to 1) the Descrimination Percent statistics for each country from HIVDescrimination.xls to GlobalHIVMerged.xlsx.
</commit_message>
<xml_diff>
--- a/GlobalHIVMerged.xlsx
+++ b/GlobalHIVMerged.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="25600" windowHeight="14580" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="2820" windowWidth="25600" windowHeight="14580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
   <si>
     <t>Country</t>
   </si>
@@ -213,6 +213,183 @@
   </si>
   <si>
     <t>Zimbabwe</t>
+  </si>
+  <si>
+    <t>60.2  (Source: DHS 2015 )</t>
+  </si>
+  <si>
+    <t>64.1  (Source: 2008 DHS)</t>
+  </si>
+  <si>
+    <t>51  (Source: INCAPSIDA 2010)</t>
+  </si>
+  <si>
+    <t>73  (Source: 2010 DHS)</t>
+  </si>
+  <si>
+    <t>30.8  (Source: Knowledge Attitudes and Practices Study 2014,)</t>
+  </si>
+  <si>
+    <t>55.4  (Source: DHS 2011-2012)</t>
+  </si>
+  <si>
+    <t>44.7  (Source: 2008-09 DHS)</t>
+  </si>
+  <si>
+    <t>57.1  (Source: 2011-12 MICS)</t>
+  </si>
+  <si>
+    <t>13.2  (Source: BAIS IV)</t>
+  </si>
+  <si>
+    <t>62.3  (Source: 2010 DHS)</t>
+  </si>
+  <si>
+    <t>25.5  (Source: 2010 DHS)</t>
+  </si>
+  <si>
+    <t>19.4  (Source: DHS 2014)</t>
+  </si>
+  <si>
+    <t>40.5  (Source: 2011 DHS)</t>
+  </si>
+  <si>
+    <t>32.6  (Source: 2010 MICS)</t>
+  </si>
+  <si>
+    <t>55.8  (Source: 2012 DHS)</t>
+  </si>
+  <si>
+    <t>35.4  (Source: 2011-12 DHS)</t>
+  </si>
+  <si>
+    <t>16.4  (Source: 2014 MICS)</t>
+  </si>
+  <si>
+    <t>44.5  (Source: 2011-12 DHS)</t>
+  </si>
+  <si>
+    <t>49.2  (Source: 2013-14 DHS )</t>
+  </si>
+  <si>
+    <t>49.3  (Source: 2013 DHS)</t>
+  </si>
+  <si>
+    <t>59.9  (Source: 2011 DHS)</t>
+  </si>
+  <si>
+    <t>25.3  (Source: 2012 DHS)</t>
+  </si>
+  <si>
+    <t>51  (Source: 2013 DHS)</t>
+  </si>
+  <si>
+    <t>67.7  (Source: 2014 DHS)</t>
+  </si>
+  <si>
+    <t>60.6  (Source: Encuesta Nacional de Salud Materno Infantil 2008-09)</t>
+  </si>
+  <si>
+    <t>80.1  (Source: 2012 DHS)</t>
+  </si>
+  <si>
+    <t>57.7  (Source: DHS 2012)</t>
+  </si>
+  <si>
+    <t>44.9  (Source: 2011-12 DHS)</t>
+  </si>
+  <si>
+    <t>62.8  (Source: 2012 DHS)</t>
+  </si>
+  <si>
+    <t>71  (Source: Knowledge Attitudes, Behaviors and Practices 2012,)</t>
+  </si>
+  <si>
+    <t>64.8  (Source: 2010-11 MICS)</t>
+  </si>
+  <si>
+    <t>11.9  (Source: 2014 DHS)</t>
+  </si>
+  <si>
+    <t>57.2  (Source: 2012 DHS)</t>
+  </si>
+  <si>
+    <t>53.5  (Source: 2011-12 MICS)</t>
+  </si>
+  <si>
+    <t>13.9  (Source: DHS 2014)</t>
+  </si>
+  <si>
+    <t>52.7  (Source: 2013 DHS)</t>
+  </si>
+  <si>
+    <t>14.9  (Source: DHS 2015-2016)</t>
+  </si>
+  <si>
+    <t>45.8  (Source: 2012-13 DHS)</t>
+  </si>
+  <si>
+    <t>75.6  (Source: 2010 MICS)</t>
+  </si>
+  <si>
+    <t>52  (Source: 2013 MICS)</t>
+  </si>
+  <si>
+    <t>28  (Source: 2011 DHS)</t>
+  </si>
+  <si>
+    <t>13  (Source: DHS 2013)</t>
+  </si>
+  <si>
+    <t>28.3  (Source: 2011 DHS)</t>
+  </si>
+  <si>
+    <t>71.5  (Source: DHS 2012)</t>
+  </si>
+  <si>
+    <t>46.8  (Source: 2013 DHS)</t>
+  </si>
+  <si>
+    <t>49  (Source: 2012-13 DHS)</t>
+  </si>
+  <si>
+    <t>70.8  (Source: 2012 MICS)</t>
+  </si>
+  <si>
+    <t>9.9  (Source: DHS 2014-2015)</t>
+  </si>
+  <si>
+    <t>84.2  (Source: OECS BSS 2005-06)</t>
+  </si>
+  <si>
+    <t>51.7  (Source: 2014 DHS)</t>
+  </si>
+  <si>
+    <t>53.4  (Source: 2013 DHS)</t>
+  </si>
+  <si>
+    <t>12.5  (Source: 2010 MICS)</t>
+  </si>
+  <si>
+    <t>63.2  (Source: 2009-10 DHS)</t>
+  </si>
+  <si>
+    <t>45.8  (Source: 2013-14 DHS )</t>
+  </si>
+  <si>
+    <t>26.2  (Source: 2011 DHS)</t>
+  </si>
+  <si>
+    <t>65.1  (Source: 2012 MICS)</t>
+  </si>
+  <si>
+    <t>26.8  (Source: 2010 DHS)</t>
+  </si>
+  <si>
+    <t>18  (Source: 2013-14 DHS )</t>
+  </si>
+  <si>
+    <t>17.8  (Source: DHS 2015 )</t>
   </si>
 </sst>
 </file>
@@ -530,7 +707,7 @@
   <dimension ref="A1:C60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -550,295 +727,472 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
+      <c r="C2" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
+      <c r="C3" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
+      <c r="C4" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
+      <c r="C5" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
+      <c r="C6" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
+      <c r="C7" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
+      <c r="C8" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
+      <c r="C9" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
+      <c r="C10" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
+      <c r="C11" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
+      <c r="C12" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>14</v>
       </c>
+      <c r="C13" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
+      <c r="C14" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
+      <c r="C15" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C28" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C29" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C30" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C31" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C32" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C33" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C34" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C35" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C36" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C37" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C38" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C39" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C40" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C41" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C42" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C43" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C44" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C45" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C46" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C47" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C48" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C49" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C50" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C51" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C52" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C53" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C54" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C55" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C56" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C57" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C58" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C59" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>61</v>
+      </c>
+      <c r="C60" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed extraneous source information from percentage values in Descrimination Percent field by finding using the regexp ' *' and replacing with nothing (1 operation, 59 records edited)
</commit_message>
<xml_diff>
--- a/GlobalHIVMerged.xlsx
+++ b/GlobalHIVMerged.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2820" windowWidth="25600" windowHeight="14580" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="25600" windowHeight="14580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>Country</t>
   </si>
@@ -213,183 +213,6 @@
   </si>
   <si>
     <t>Zimbabwe</t>
-  </si>
-  <si>
-    <t>60.2  (Source: DHS 2015 )</t>
-  </si>
-  <si>
-    <t>64.1  (Source: 2008 DHS)</t>
-  </si>
-  <si>
-    <t>51  (Source: INCAPSIDA 2010)</t>
-  </si>
-  <si>
-    <t>73  (Source: 2010 DHS)</t>
-  </si>
-  <si>
-    <t>30.8  (Source: Knowledge Attitudes and Practices Study 2014,)</t>
-  </si>
-  <si>
-    <t>55.4  (Source: DHS 2011-2012)</t>
-  </si>
-  <si>
-    <t>44.7  (Source: 2008-09 DHS)</t>
-  </si>
-  <si>
-    <t>57.1  (Source: 2011-12 MICS)</t>
-  </si>
-  <si>
-    <t>13.2  (Source: BAIS IV)</t>
-  </si>
-  <si>
-    <t>62.3  (Source: 2010 DHS)</t>
-  </si>
-  <si>
-    <t>25.5  (Source: 2010 DHS)</t>
-  </si>
-  <si>
-    <t>19.4  (Source: DHS 2014)</t>
-  </si>
-  <si>
-    <t>40.5  (Source: 2011 DHS)</t>
-  </si>
-  <si>
-    <t>32.6  (Source: 2010 MICS)</t>
-  </si>
-  <si>
-    <t>55.8  (Source: 2012 DHS)</t>
-  </si>
-  <si>
-    <t>35.4  (Source: 2011-12 DHS)</t>
-  </si>
-  <si>
-    <t>16.4  (Source: 2014 MICS)</t>
-  </si>
-  <si>
-    <t>44.5  (Source: 2011-12 DHS)</t>
-  </si>
-  <si>
-    <t>49.2  (Source: 2013-14 DHS )</t>
-  </si>
-  <si>
-    <t>49.3  (Source: 2013 DHS)</t>
-  </si>
-  <si>
-    <t>59.9  (Source: 2011 DHS)</t>
-  </si>
-  <si>
-    <t>25.3  (Source: 2012 DHS)</t>
-  </si>
-  <si>
-    <t>51  (Source: 2013 DHS)</t>
-  </si>
-  <si>
-    <t>67.7  (Source: 2014 DHS)</t>
-  </si>
-  <si>
-    <t>60.6  (Source: Encuesta Nacional de Salud Materno Infantil 2008-09)</t>
-  </si>
-  <si>
-    <t>80.1  (Source: 2012 DHS)</t>
-  </si>
-  <si>
-    <t>57.7  (Source: DHS 2012)</t>
-  </si>
-  <si>
-    <t>44.9  (Source: 2011-12 DHS)</t>
-  </si>
-  <si>
-    <t>62.8  (Source: 2012 DHS)</t>
-  </si>
-  <si>
-    <t>71  (Source: Knowledge Attitudes, Behaviors and Practices 2012,)</t>
-  </si>
-  <si>
-    <t>64.8  (Source: 2010-11 MICS)</t>
-  </si>
-  <si>
-    <t>11.9  (Source: 2014 DHS)</t>
-  </si>
-  <si>
-    <t>57.2  (Source: 2012 DHS)</t>
-  </si>
-  <si>
-    <t>53.5  (Source: 2011-12 MICS)</t>
-  </si>
-  <si>
-    <t>13.9  (Source: DHS 2014)</t>
-  </si>
-  <si>
-    <t>52.7  (Source: 2013 DHS)</t>
-  </si>
-  <si>
-    <t>14.9  (Source: DHS 2015-2016)</t>
-  </si>
-  <si>
-    <t>45.8  (Source: 2012-13 DHS)</t>
-  </si>
-  <si>
-    <t>75.6  (Source: 2010 MICS)</t>
-  </si>
-  <si>
-    <t>52  (Source: 2013 MICS)</t>
-  </si>
-  <si>
-    <t>28  (Source: 2011 DHS)</t>
-  </si>
-  <si>
-    <t>13  (Source: DHS 2013)</t>
-  </si>
-  <si>
-    <t>28.3  (Source: 2011 DHS)</t>
-  </si>
-  <si>
-    <t>71.5  (Source: DHS 2012)</t>
-  </si>
-  <si>
-    <t>46.8  (Source: 2013 DHS)</t>
-  </si>
-  <si>
-    <t>49  (Source: 2012-13 DHS)</t>
-  </si>
-  <si>
-    <t>70.8  (Source: 2012 MICS)</t>
-  </si>
-  <si>
-    <t>9.9  (Source: DHS 2014-2015)</t>
-  </si>
-  <si>
-    <t>84.2  (Source: OECS BSS 2005-06)</t>
-  </si>
-  <si>
-    <t>51.7  (Source: 2014 DHS)</t>
-  </si>
-  <si>
-    <t>53.4  (Source: 2013 DHS)</t>
-  </si>
-  <si>
-    <t>12.5  (Source: 2010 MICS)</t>
-  </si>
-  <si>
-    <t>63.2  (Source: 2009-10 DHS)</t>
-  </si>
-  <si>
-    <t>45.8  (Source: 2013-14 DHS )</t>
-  </si>
-  <si>
-    <t>26.2  (Source: 2011 DHS)</t>
-  </si>
-  <si>
-    <t>65.1  (Source: 2012 MICS)</t>
-  </si>
-  <si>
-    <t>26.8  (Source: 2010 DHS)</t>
-  </si>
-  <si>
-    <t>18  (Source: 2013-14 DHS )</t>
-  </si>
-  <si>
-    <t>17.8  (Source: DHS 2015 )</t>
   </si>
 </sst>
 </file>
@@ -707,7 +530,7 @@
   <dimension ref="A1:C60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -727,472 +550,472 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>62</v>
+      <c r="C2">
+        <v>60.2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
-        <v>63</v>
+      <c r="C3">
+        <v>64.099999999999994</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
-        <v>64</v>
+      <c r="C4">
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
-        <v>65</v>
+      <c r="C5">
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" t="s">
-        <v>66</v>
+      <c r="C6">
+        <v>30.8</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="C7" t="s">
-        <v>67</v>
+      <c r="C7">
+        <v>55.4</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="C8" t="s">
-        <v>68</v>
+      <c r="C8">
+        <v>44.7</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="C9" t="s">
-        <v>69</v>
+      <c r="C9">
+        <v>57.1</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="C10" t="s">
-        <v>70</v>
+      <c r="C10">
+        <v>13.2</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="C11" t="s">
-        <v>71</v>
+      <c r="C11">
+        <v>62.3</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="C12" t="s">
-        <v>72</v>
+      <c r="C12">
+        <v>25.5</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>14</v>
       </c>
-      <c r="C13" t="s">
-        <v>73</v>
+      <c r="C13">
+        <v>19.399999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="C14" t="s">
-        <v>74</v>
+      <c r="C14">
+        <v>40.5</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
-      <c r="C15" t="s">
-        <v>75</v>
+      <c r="C15">
+        <v>32.6</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
-      <c r="C16" t="s">
-        <v>76</v>
+      <c r="C16">
+        <v>55.8</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>18</v>
       </c>
-      <c r="C17" t="s">
-        <v>77</v>
+      <c r="C17">
+        <v>35.4</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>19</v>
       </c>
-      <c r="C18" t="s">
-        <v>78</v>
+      <c r="C18">
+        <v>16.399999999999999</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>20</v>
       </c>
-      <c r="C19" t="s">
-        <v>79</v>
+      <c r="C19">
+        <v>44.5</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>21</v>
       </c>
-      <c r="C20" t="s">
-        <v>80</v>
+      <c r="C20">
+        <v>49.2</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>22</v>
       </c>
-      <c r="C21" t="s">
-        <v>81</v>
+      <c r="C21">
+        <v>49.3</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>23</v>
       </c>
-      <c r="C22" t="s">
-        <v>82</v>
+      <c r="C22">
+        <v>59.9</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>24</v>
       </c>
-      <c r="C23" t="s">
-        <v>83</v>
+      <c r="C23">
+        <v>25.3</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>25</v>
       </c>
-      <c r="C24" t="s">
-        <v>84</v>
+      <c r="C24">
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>26</v>
       </c>
-      <c r="C25" t="s">
-        <v>85</v>
+      <c r="C25">
+        <v>67.7</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>27</v>
       </c>
-      <c r="C26" t="s">
-        <v>86</v>
+      <c r="C26">
+        <v>60.6</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>28</v>
       </c>
-      <c r="C27" t="s">
-        <v>87</v>
+      <c r="C27">
+        <v>80.099999999999994</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>29</v>
       </c>
-      <c r="C28" t="s">
-        <v>88</v>
+      <c r="C28">
+        <v>57.7</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>30</v>
       </c>
-      <c r="C29" t="s">
-        <v>89</v>
+      <c r="C29">
+        <v>44.9</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>31</v>
       </c>
-      <c r="C30" t="s">
-        <v>90</v>
+      <c r="C30">
+        <v>62.8</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>32</v>
       </c>
-      <c r="C31" t="s">
-        <v>91</v>
+      <c r="C31">
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>33</v>
       </c>
-      <c r="C32" t="s">
-        <v>92</v>
+      <c r="C32">
+        <v>64.8</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>34</v>
       </c>
-      <c r="C33" t="s">
-        <v>93</v>
+      <c r="C33">
+        <v>11.9</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>35</v>
       </c>
-      <c r="C34" t="s">
-        <v>94</v>
+      <c r="C34">
+        <v>57.2</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>36</v>
       </c>
-      <c r="C35" t="s">
-        <v>95</v>
+      <c r="C35">
+        <v>53.5</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>37</v>
       </c>
-      <c r="C36" t="s">
-        <v>96</v>
+      <c r="C36">
+        <v>13.9</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>38</v>
       </c>
-      <c r="C37" t="s">
-        <v>97</v>
+      <c r="C37">
+        <v>52.7</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>39</v>
       </c>
-      <c r="C38" t="s">
-        <v>98</v>
+      <c r="C38">
+        <v>14.9</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>40</v>
       </c>
-      <c r="C39" t="s">
-        <v>99</v>
+      <c r="C39">
+        <v>45.8</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>41</v>
       </c>
-      <c r="C40" t="s">
-        <v>100</v>
+      <c r="C40">
+        <v>75.599999999999994</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>42</v>
       </c>
-      <c r="C41" t="s">
-        <v>101</v>
+      <c r="C41">
+        <v>52</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>43</v>
       </c>
-      <c r="C42" t="s">
-        <v>102</v>
+      <c r="C42">
+        <v>28</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>44</v>
       </c>
-      <c r="C43" t="s">
-        <v>103</v>
+      <c r="C43">
+        <v>13</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>45</v>
       </c>
-      <c r="C44" t="s">
-        <v>104</v>
+      <c r="C44">
+        <v>28.3</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>46</v>
       </c>
-      <c r="C45" t="s">
-        <v>105</v>
+      <c r="C45">
+        <v>71.5</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>47</v>
       </c>
-      <c r="C46" t="s">
-        <v>106</v>
+      <c r="C46">
+        <v>46.8</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>48</v>
       </c>
-      <c r="C47" t="s">
-        <v>107</v>
+      <c r="C47">
+        <v>49</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>49</v>
       </c>
-      <c r="C48" t="s">
-        <v>108</v>
+      <c r="C48">
+        <v>70.8</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>50</v>
       </c>
-      <c r="C49" t="s">
-        <v>109</v>
+      <c r="C49">
+        <v>9.9</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>51</v>
       </c>
-      <c r="C50" t="s">
-        <v>110</v>
+      <c r="C50">
+        <v>84.2</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>52</v>
       </c>
-      <c r="C51" t="s">
-        <v>111</v>
+      <c r="C51">
+        <v>51.7</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>53</v>
       </c>
-      <c r="C52" t="s">
-        <v>112</v>
+      <c r="C52">
+        <v>53.4</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>54</v>
       </c>
-      <c r="C53" t="s">
-        <v>113</v>
+      <c r="C53">
+        <v>12.5</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>55</v>
       </c>
-      <c r="C54" t="s">
-        <v>114</v>
+      <c r="C54">
+        <v>63.2</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>56</v>
       </c>
-      <c r="C55" t="s">
-        <v>115</v>
+      <c r="C55">
+        <v>45.8</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>57</v>
       </c>
-      <c r="C56" t="s">
-        <v>116</v>
+      <c r="C56">
+        <v>26.2</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>58</v>
       </c>
-      <c r="C57" t="s">
-        <v>117</v>
+      <c r="C57">
+        <v>65.099999999999994</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>59</v>
       </c>
-      <c r="C58" t="s">
-        <v>118</v>
+      <c r="C58">
+        <v>26.8</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>60</v>
       </c>
-      <c r="C59" t="s">
-        <v>119</v>
+      <c r="C59">
+        <v>18</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>61</v>
       </c>
-      <c r="C60" t="s">
-        <v>120</v>
+      <c r="C60">
+        <v>17.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added attribute to merged file of 'Country (Population)' to make copying and pasting HIV population values matching countries easier.
</commit_message>
<xml_diff>
--- a/GlobalHIVMerged.xlsx
+++ b/GlobalHIVMerged.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="25600" windowHeight="14580" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>Country</t>
   </si>
@@ -213,6 +213,9 @@
   </si>
   <si>
     <t>Zimbabwe</t>
+  </si>
+  <si>
+    <t>Country (Population)</t>
   </si>
 </sst>
 </file>
@@ -527,494 +530,497 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C60"/>
+  <dimension ref="A1:D60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>60.2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>64.099999999999994</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>30.8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>55.4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>44.7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>57.1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>13.2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>62.3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>25.5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>14</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>19.399999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>40.5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>32.6</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>55.8</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>18</v>
       </c>
-      <c r="C17">
+      <c r="D17">
         <v>35.4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>19</v>
       </c>
-      <c r="C18">
+      <c r="D18">
         <v>16.399999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>20</v>
       </c>
-      <c r="C19">
+      <c r="D19">
         <v>44.5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>21</v>
       </c>
-      <c r="C20">
+      <c r="D20">
         <v>49.2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>22</v>
       </c>
-      <c r="C21">
+      <c r="D21">
         <v>49.3</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>23</v>
       </c>
-      <c r="C22">
+      <c r="D22">
         <v>59.9</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>24</v>
       </c>
-      <c r="C23">
+      <c r="D23">
         <v>25.3</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>25</v>
       </c>
-      <c r="C24">
+      <c r="D24">
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>26</v>
       </c>
-      <c r="C25">
+      <c r="D25">
         <v>67.7</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>27</v>
       </c>
-      <c r="C26">
+      <c r="D26">
         <v>60.6</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>28</v>
       </c>
-      <c r="C27">
+      <c r="D27">
         <v>80.099999999999994</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>29</v>
       </c>
-      <c r="C28">
+      <c r="D28">
         <v>57.7</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>30</v>
       </c>
-      <c r="C29">
+      <c r="D29">
         <v>44.9</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>31</v>
       </c>
-      <c r="C30">
+      <c r="D30">
         <v>62.8</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>32</v>
       </c>
-      <c r="C31">
+      <c r="D31">
         <v>71</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>33</v>
       </c>
-      <c r="C32">
+      <c r="D32">
         <v>64.8</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>34</v>
       </c>
-      <c r="C33">
+      <c r="D33">
         <v>11.9</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>35</v>
       </c>
-      <c r="C34">
+      <c r="D34">
         <v>57.2</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>36</v>
       </c>
-      <c r="C35">
+      <c r="D35">
         <v>53.5</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>37</v>
       </c>
-      <c r="C36">
+      <c r="D36">
         <v>13.9</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>38</v>
       </c>
-      <c r="C37">
+      <c r="D37">
         <v>52.7</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>39</v>
       </c>
-      <c r="C38">
+      <c r="D38">
         <v>14.9</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>40</v>
       </c>
-      <c r="C39">
+      <c r="D39">
         <v>45.8</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>41</v>
       </c>
-      <c r="C40">
+      <c r="D40">
         <v>75.599999999999994</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>42</v>
       </c>
-      <c r="C41">
+      <c r="D41">
         <v>52</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>43</v>
       </c>
-      <c r="C42">
+      <c r="D42">
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>44</v>
       </c>
-      <c r="C43">
+      <c r="D43">
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>45</v>
       </c>
-      <c r="C44">
+      <c r="D44">
         <v>28.3</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>46</v>
       </c>
-      <c r="C45">
+      <c r="D45">
         <v>71.5</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>47</v>
       </c>
-      <c r="C46">
+      <c r="D46">
         <v>46.8</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>48</v>
       </c>
-      <c r="C47">
+      <c r="D47">
         <v>49</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>49</v>
       </c>
-      <c r="C48">
+      <c r="D48">
         <v>70.8</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>50</v>
       </c>
-      <c r="C49">
+      <c r="D49">
         <v>9.9</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>51</v>
       </c>
-      <c r="C50">
+      <c r="D50">
         <v>84.2</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>52</v>
       </c>
-      <c r="C51">
+      <c r="D51">
         <v>51.7</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>53</v>
       </c>
-      <c r="C52">
+      <c r="D52">
         <v>53.4</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>54</v>
       </c>
-      <c r="C53">
+      <c r="D53">
         <v>12.5</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>55</v>
       </c>
-      <c r="C54">
+      <c r="D54">
         <v>63.2</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>56</v>
       </c>
-      <c r="C55">
+      <c r="D55">
         <v>45.8</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>57</v>
       </c>
-      <c r="C56">
+      <c r="D56">
         <v>26.2</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>58</v>
       </c>
-      <c r="C57">
+      <c r="D57">
         <v>65.099999999999994</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>59</v>
       </c>
-      <c r="C58">
+      <c r="D58">
         <v>26.8</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>60</v>
       </c>
-      <c r="C59">
+      <c r="D59">
         <v>18</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>61</v>
       </c>
-      <c r="C60">
+      <c r="D60">
         <v>17.8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Did not add before last change, recommitting.
</commit_message>
<xml_diff>
--- a/GlobalHIVMerged.xlsx
+++ b/GlobalHIVMerged.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="174">
   <si>
     <t>Country</t>
   </si>
@@ -216,6 +216,339 @@
   </si>
   <si>
     <t>Country (Population)</t>
+  </si>
+  <si>
+    <t>Algeria</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Austria</t>
+  </si>
+  <si>
+    <t>Azerbaijan</t>
+  </si>
+  <si>
+    <t>Bahamas</t>
+  </si>
+  <si>
+    <t>Bahrain</t>
+  </si>
+  <si>
+    <t>Bangladesh</t>
+  </si>
+  <si>
+    <t>Barbados</t>
+  </si>
+  <si>
+    <t>Belarus</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>Bhutan</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>Brunei Darussalam</t>
+  </si>
+  <si>
+    <t>Bulgaria</t>
+  </si>
+  <si>
+    <t>Cabo Verde</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>Chad</t>
+  </si>
+  <si>
+    <t>Chile</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Colombia</t>
+  </si>
+  <si>
+    <t>Costa Rica</t>
+  </si>
+  <si>
+    <t>Croatia</t>
+  </si>
+  <si>
+    <t>Cyprus</t>
+  </si>
+  <si>
+    <t>Czech Republic</t>
+  </si>
+  <si>
+    <t>Democratic People's Republic of Korea</t>
+  </si>
+  <si>
+    <t>Denmark</t>
+  </si>
+  <si>
+    <t>Djibouti</t>
+  </si>
+  <si>
+    <t>Ecuador</t>
+  </si>
+  <si>
+    <t>Egypt</t>
+  </si>
+  <si>
+    <t>El Salvador</t>
+  </si>
+  <si>
+    <t>Equatorial Guinea</t>
+  </si>
+  <si>
+    <t>Eritrea</t>
+  </si>
+  <si>
+    <t>Estonia</t>
+  </si>
+  <si>
+    <t>Fiji</t>
+  </si>
+  <si>
+    <t>Finland</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Greece</t>
+  </si>
+  <si>
+    <t>Guinea-Bissau</t>
+  </si>
+  <si>
+    <t>Guyana</t>
+  </si>
+  <si>
+    <t>Hungary</t>
+  </si>
+  <si>
+    <t>Iceland</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Iran (Islamic Republic of)</t>
+  </si>
+  <si>
+    <t>Ireland</t>
+  </si>
+  <si>
+    <t>Israel</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>Jordan</t>
+  </si>
+  <si>
+    <t>Kuwait</t>
+  </si>
+  <si>
+    <t>Latvia</t>
+  </si>
+  <si>
+    <t>Lebanon</t>
+  </si>
+  <si>
+    <t>Lithuania</t>
+  </si>
+  <si>
+    <t>Luxembourg</t>
+  </si>
+  <si>
+    <t>Madagascar</t>
+  </si>
+  <si>
+    <t>Malaysia</t>
+  </si>
+  <si>
+    <t>Maldives</t>
+  </si>
+  <si>
+    <t>Malta</t>
+  </si>
+  <si>
+    <t>Mauritania</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Morocco</t>
+  </si>
+  <si>
+    <t>Myanmar</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>New Zealand</t>
+  </si>
+  <si>
+    <t>Nicaragua</t>
+  </si>
+  <si>
+    <t>Norway</t>
+  </si>
+  <si>
+    <t>Oman</t>
+  </si>
+  <si>
+    <t>Panama</t>
+  </si>
+  <si>
+    <t>Papua New Guinea</t>
+  </si>
+  <si>
+    <t>Paraguay</t>
+  </si>
+  <si>
+    <t>Peru</t>
+  </si>
+  <si>
+    <t>Philippines</t>
+  </si>
+  <si>
+    <t>Poland</t>
+  </si>
+  <si>
+    <t>Portugal</t>
+  </si>
+  <si>
+    <t>Qatar</t>
+  </si>
+  <si>
+    <t>Republic of Korea</t>
+  </si>
+  <si>
+    <t>Romania</t>
+  </si>
+  <si>
+    <t>Russian Federation</t>
+  </si>
+  <si>
+    <t>Saudi Arabia</t>
+  </si>
+  <si>
+    <t>Serbia</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>Slovakia</t>
+  </si>
+  <si>
+    <t>Slovenia</t>
+  </si>
+  <si>
+    <t>Somalia</t>
+  </si>
+  <si>
+    <t>South Africa</t>
+  </si>
+  <si>
+    <t>South Sudan</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>Sri Lanka</t>
+  </si>
+  <si>
+    <t>Sudan</t>
+  </si>
+  <si>
+    <t>Suriname</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>Syrian Arab Republic</t>
+  </si>
+  <si>
+    <t>Tajikistan</t>
+  </si>
+  <si>
+    <t>Thailand</t>
+  </si>
+  <si>
+    <t>The former Yugoslav Republic of Macedonia</t>
+  </si>
+  <si>
+    <t>Trinidad and Tobago</t>
+  </si>
+  <si>
+    <t>Tunisia</t>
+  </si>
+  <si>
+    <t>Turkey</t>
+  </si>
+  <si>
+    <t>Turkmenistan</t>
+  </si>
+  <si>
+    <t>United Arab Emirates</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>Uruguay</t>
+  </si>
+  <si>
+    <t>Uzbekistan</t>
+  </si>
+  <si>
+    <t>Venezuela (Bolivarian Republic of)</t>
+  </si>
+  <si>
+    <t>Viet Nam</t>
+  </si>
+  <si>
+    <t>Yemen</t>
+  </si>
+  <si>
+    <t>Global</t>
   </si>
 </sst>
 </file>
@@ -530,10 +863,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:D170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -556,6 +889,9 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
       <c r="D2">
         <v>60.2</v>
       </c>
@@ -564,6 +900,9 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
       <c r="D3">
         <v>64.099999999999994</v>
       </c>
@@ -572,6 +911,9 @@
       <c r="A4" t="s">
         <v>5</v>
       </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
       <c r="D4">
         <v>51</v>
       </c>
@@ -580,6 +922,9 @@
       <c r="A5" t="s">
         <v>6</v>
       </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
       <c r="D5">
         <v>73</v>
       </c>
@@ -588,6 +933,9 @@
       <c r="A6" t="s">
         <v>7</v>
       </c>
+      <c r="B6" t="s">
+        <v>64</v>
+      </c>
       <c r="D6">
         <v>30.8</v>
       </c>
@@ -596,6 +944,9 @@
       <c r="A7" t="s">
         <v>8</v>
       </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
       <c r="D7">
         <v>55.4</v>
       </c>
@@ -604,6 +955,9 @@
       <c r="A8" t="s">
         <v>9</v>
       </c>
+      <c r="B8" t="s">
+        <v>65</v>
+      </c>
       <c r="D8">
         <v>44.7</v>
       </c>
@@ -612,6 +966,9 @@
       <c r="A9" t="s">
         <v>10</v>
       </c>
+      <c r="B9" t="s">
+        <v>66</v>
+      </c>
       <c r="D9">
         <v>57.1</v>
       </c>
@@ -620,6 +977,9 @@
       <c r="A10" t="s">
         <v>11</v>
       </c>
+      <c r="B10" t="s">
+        <v>67</v>
+      </c>
       <c r="D10">
         <v>13.2</v>
       </c>
@@ -628,6 +988,9 @@
       <c r="A11" t="s">
         <v>12</v>
       </c>
+      <c r="B11" t="s">
+        <v>68</v>
+      </c>
       <c r="D11">
         <v>62.3</v>
       </c>
@@ -636,6 +999,9 @@
       <c r="A12" t="s">
         <v>13</v>
       </c>
+      <c r="B12" t="s">
+        <v>69</v>
+      </c>
       <c r="D12">
         <v>25.5</v>
       </c>
@@ -644,6 +1010,9 @@
       <c r="A13" t="s">
         <v>14</v>
       </c>
+      <c r="B13" t="s">
+        <v>70</v>
+      </c>
       <c r="D13">
         <v>19.399999999999999</v>
       </c>
@@ -652,6 +1021,9 @@
       <c r="A14" t="s">
         <v>15</v>
       </c>
+      <c r="B14" t="s">
+        <v>71</v>
+      </c>
       <c r="D14">
         <v>40.5</v>
       </c>
@@ -660,6 +1032,9 @@
       <c r="A15" t="s">
         <v>16</v>
       </c>
+      <c r="B15" t="s">
+        <v>72</v>
+      </c>
       <c r="D15">
         <v>32.6</v>
       </c>
@@ -668,6 +1043,9 @@
       <c r="A16" t="s">
         <v>17</v>
       </c>
+      <c r="B16" t="s">
+        <v>73</v>
+      </c>
       <c r="D16">
         <v>55.8</v>
       </c>
@@ -676,6 +1054,9 @@
       <c r="A17" t="s">
         <v>18</v>
       </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
       <c r="D17">
         <v>35.4</v>
       </c>
@@ -684,6 +1065,9 @@
       <c r="A18" t="s">
         <v>19</v>
       </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
       <c r="D18">
         <v>16.399999999999999</v>
       </c>
@@ -692,6 +1076,9 @@
       <c r="A19" t="s">
         <v>20</v>
       </c>
+      <c r="B19" t="s">
+        <v>74</v>
+      </c>
       <c r="D19">
         <v>44.5</v>
       </c>
@@ -700,6 +1087,9 @@
       <c r="A20" t="s">
         <v>21</v>
       </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
       <c r="D20">
         <v>49.2</v>
       </c>
@@ -708,6 +1098,9 @@
       <c r="A21" t="s">
         <v>22</v>
       </c>
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
       <c r="D21">
         <v>49.3</v>
       </c>
@@ -716,6 +1109,9 @@
       <c r="A22" t="s">
         <v>23</v>
       </c>
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
       <c r="D22">
         <v>59.9</v>
       </c>
@@ -724,6 +1120,9 @@
       <c r="A23" t="s">
         <v>24</v>
       </c>
+      <c r="B23" t="s">
+        <v>75</v>
+      </c>
       <c r="D23">
         <v>25.3</v>
       </c>
@@ -732,6 +1131,9 @@
       <c r="A24" t="s">
         <v>25</v>
       </c>
+      <c r="B24" t="s">
+        <v>76</v>
+      </c>
       <c r="D24">
         <v>51</v>
       </c>
@@ -740,6 +1142,9 @@
       <c r="A25" t="s">
         <v>26</v>
       </c>
+      <c r="B25" t="s">
+        <v>77</v>
+      </c>
       <c r="D25">
         <v>67.7</v>
       </c>
@@ -748,6 +1153,9 @@
       <c r="A26" t="s">
         <v>27</v>
       </c>
+      <c r="B26" t="s">
+        <v>12</v>
+      </c>
       <c r="D26">
         <v>60.6</v>
       </c>
@@ -756,6 +1164,9 @@
       <c r="A27" t="s">
         <v>28</v>
       </c>
+      <c r="B27" t="s">
+        <v>13</v>
+      </c>
       <c r="D27">
         <v>80.099999999999994</v>
       </c>
@@ -764,6 +1175,9 @@
       <c r="A28" t="s">
         <v>29</v>
       </c>
+      <c r="B28" t="s">
+        <v>78</v>
+      </c>
       <c r="D28">
         <v>57.7</v>
       </c>
@@ -772,6 +1186,9 @@
       <c r="A29" t="s">
         <v>30</v>
       </c>
+      <c r="B29" t="s">
+        <v>14</v>
+      </c>
       <c r="D29">
         <v>44.9</v>
       </c>
@@ -780,6 +1197,9 @@
       <c r="A30" t="s">
         <v>31</v>
       </c>
+      <c r="B30" t="s">
+        <v>15</v>
+      </c>
       <c r="D30">
         <v>62.8</v>
       </c>
@@ -788,6 +1208,9 @@
       <c r="A31" t="s">
         <v>32</v>
       </c>
+      <c r="B31" t="s">
+        <v>79</v>
+      </c>
       <c r="D31">
         <v>71</v>
       </c>
@@ -796,6 +1219,9 @@
       <c r="A32" t="s">
         <v>33</v>
       </c>
+      <c r="B32" t="s">
+        <v>16</v>
+      </c>
       <c r="D32">
         <v>64.8</v>
       </c>
@@ -804,6 +1230,9 @@
       <c r="A33" t="s">
         <v>34</v>
       </c>
+      <c r="B33" t="s">
+        <v>80</v>
+      </c>
       <c r="D33">
         <v>11.9</v>
       </c>
@@ -812,6 +1241,9 @@
       <c r="A34" t="s">
         <v>35</v>
       </c>
+      <c r="B34" t="s">
+        <v>81</v>
+      </c>
       <c r="D34">
         <v>57.2</v>
       </c>
@@ -820,6 +1252,9 @@
       <c r="A35" t="s">
         <v>36</v>
       </c>
+      <c r="B35" t="s">
+        <v>82</v>
+      </c>
       <c r="D35">
         <v>53.5</v>
       </c>
@@ -828,6 +1263,9 @@
       <c r="A36" t="s">
         <v>37</v>
       </c>
+      <c r="B36" t="s">
+        <v>83</v>
+      </c>
       <c r="D36">
         <v>13.9</v>
       </c>
@@ -836,6 +1274,9 @@
       <c r="A37" t="s">
         <v>38</v>
       </c>
+      <c r="B37" t="s">
+        <v>17</v>
+      </c>
       <c r="D37">
         <v>52.7</v>
       </c>
@@ -844,6 +1285,9 @@
       <c r="A38" t="s">
         <v>39</v>
       </c>
+      <c r="B38" t="s">
+        <v>18</v>
+      </c>
       <c r="D38">
         <v>14.9</v>
       </c>
@@ -852,6 +1296,9 @@
       <c r="A39" t="s">
         <v>40</v>
       </c>
+      <c r="B39" t="s">
+        <v>84</v>
+      </c>
       <c r="D39">
         <v>45.8</v>
       </c>
@@ -860,6 +1307,9 @@
       <c r="A40" t="s">
         <v>41</v>
       </c>
+      <c r="B40" t="s">
+        <v>85</v>
+      </c>
       <c r="D40">
         <v>75.599999999999994</v>
       </c>
@@ -868,6 +1318,9 @@
       <c r="A41" t="s">
         <v>42</v>
       </c>
+      <c r="B41" t="s">
+        <v>19</v>
+      </c>
       <c r="D41">
         <v>52</v>
       </c>
@@ -876,6 +1329,9 @@
       <c r="A42" t="s">
         <v>43</v>
       </c>
+      <c r="B42" t="s">
+        <v>86</v>
+      </c>
       <c r="D42">
         <v>28</v>
       </c>
@@ -884,6 +1340,9 @@
       <c r="A43" t="s">
         <v>44</v>
       </c>
+      <c r="B43" t="s">
+        <v>87</v>
+      </c>
       <c r="D43">
         <v>13</v>
       </c>
@@ -892,6 +1351,9 @@
       <c r="A44" t="s">
         <v>45</v>
       </c>
+      <c r="B44" t="s">
+        <v>20</v>
+      </c>
       <c r="D44">
         <v>28.3</v>
       </c>
@@ -900,6 +1362,9 @@
       <c r="A45" t="s">
         <v>46</v>
       </c>
+      <c r="B45" t="s">
+        <v>88</v>
+      </c>
       <c r="D45">
         <v>71.5</v>
       </c>
@@ -908,6 +1373,9 @@
       <c r="A46" t="s">
         <v>47</v>
       </c>
+      <c r="B46" t="s">
+        <v>21</v>
+      </c>
       <c r="D46">
         <v>46.8</v>
       </c>
@@ -916,6 +1384,9 @@
       <c r="A47" t="s">
         <v>48</v>
       </c>
+      <c r="B47" t="s">
+        <v>89</v>
+      </c>
       <c r="D47">
         <v>49</v>
       </c>
@@ -924,6 +1395,9 @@
       <c r="A48" t="s">
         <v>49</v>
       </c>
+      <c r="B48" t="s">
+        <v>90</v>
+      </c>
       <c r="D48">
         <v>70.8</v>
       </c>
@@ -932,6 +1406,9 @@
       <c r="A49" t="s">
         <v>50</v>
       </c>
+      <c r="B49" t="s">
+        <v>22</v>
+      </c>
       <c r="D49">
         <v>9.9</v>
       </c>
@@ -940,6 +1417,9 @@
       <c r="A50" t="s">
         <v>51</v>
       </c>
+      <c r="B50" t="s">
+        <v>91</v>
+      </c>
       <c r="D50">
         <v>84.2</v>
       </c>
@@ -948,6 +1428,9 @@
       <c r="A51" t="s">
         <v>52</v>
       </c>
+      <c r="B51" t="s">
+        <v>92</v>
+      </c>
       <c r="D51">
         <v>51.7</v>
       </c>
@@ -956,6 +1439,9 @@
       <c r="A52" t="s">
         <v>53</v>
       </c>
+      <c r="B52" t="s">
+        <v>93</v>
+      </c>
       <c r="D52">
         <v>53.4</v>
       </c>
@@ -964,6 +1450,9 @@
       <c r="A53" t="s">
         <v>54</v>
       </c>
+      <c r="B53" t="s">
+        <v>94</v>
+      </c>
       <c r="D53">
         <v>12.5</v>
       </c>
@@ -972,6 +1461,9 @@
       <c r="A54" t="s">
         <v>55</v>
       </c>
+      <c r="B54" t="s">
+        <v>95</v>
+      </c>
       <c r="D54">
         <v>63.2</v>
       </c>
@@ -980,6 +1472,9 @@
       <c r="A55" t="s">
         <v>56</v>
       </c>
+      <c r="B55" t="s">
+        <v>96</v>
+      </c>
       <c r="D55">
         <v>45.8</v>
       </c>
@@ -988,6 +1483,9 @@
       <c r="A56" t="s">
         <v>57</v>
       </c>
+      <c r="B56" t="s">
+        <v>23</v>
+      </c>
       <c r="D56">
         <v>26.2</v>
       </c>
@@ -996,6 +1494,9 @@
       <c r="A57" t="s">
         <v>58</v>
       </c>
+      <c r="B57" t="s">
+        <v>97</v>
+      </c>
       <c r="D57">
         <v>65.099999999999994</v>
       </c>
@@ -1004,6 +1505,9 @@
       <c r="A58" t="s">
         <v>59</v>
       </c>
+      <c r="B58" t="s">
+        <v>98</v>
+      </c>
       <c r="D58">
         <v>26.8</v>
       </c>
@@ -1012,6 +1516,9 @@
       <c r="A59" t="s">
         <v>60</v>
       </c>
+      <c r="B59" t="s">
+        <v>99</v>
+      </c>
       <c r="D59">
         <v>18</v>
       </c>
@@ -1020,8 +1527,561 @@
       <c r="A60" t="s">
         <v>61</v>
       </c>
+      <c r="B60" t="s">
+        <v>24</v>
+      </c>
       <c r="D60">
         <v>17.8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B61" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B62" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B63" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B64" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B65" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B66" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B67" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B68" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B69" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B70" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B71" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B72" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B73" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B74" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B75" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B76" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B77" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B78" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B79" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B80" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B81" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B82" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B83" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B84" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B85" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B86" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B87" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B88" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B89" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B90" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B91" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B92" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B93" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B94" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B95" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="96" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B96" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B97" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B98" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="99" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B99" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="100" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B100" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="101" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B101" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="102" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B102" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="103" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B103" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="104" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B104" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="105" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B105" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="106" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B106" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="107" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B107" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="108" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B108" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="109" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B109" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="110" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B110" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="111" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B111" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="112" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B112" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="113" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B113" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="114" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B114" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="115" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B115" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="116" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B116" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="117" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B117" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="118" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B118" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="119" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B119" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="120" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B120" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="121" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B121" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="122" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B122" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="123" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B123" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="124" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B124" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="125" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B125" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="126" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B126" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="127" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B127" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="128" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B128" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="129" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B129" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="130" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B130" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="131" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B131" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="132" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B132" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="133" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B133" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="134" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B134" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="135" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B135" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="136" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B136" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="137" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B137" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="138" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B138" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="139" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B139" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="140" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B140" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="141" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B141" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="142" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B142" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="143" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B143" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="144" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B144" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="145" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B145" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="146" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B146" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="147" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B147" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="148" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B148" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="149" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B149" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="150" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B150" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="151" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B151" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="152" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B152" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="153" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B153" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="154" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B154" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="155" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B155" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="156" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B156" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="157" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B157" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="158" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B158" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="159" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B159" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="160" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B160" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="161" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B161" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="162" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B162" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="163" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B163" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="164" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B164" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="165" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B165" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="166" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B166" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="167" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B167" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="168" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B168" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="169" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B169" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="170" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B170" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Copy and pasted (1 to 1) ‘2016’ from HIVPopulation to ‘Number of People Living with HIV’ in GlobalHIVMerged
</commit_message>
<xml_diff>
--- a/GlobalHIVMerged.xlsx
+++ b/GlobalHIVMerged.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="300">
   <si>
     <t>Country</t>
   </si>
@@ -549,6 +549,384 @@
   </si>
   <si>
     <t>Global</t>
+  </si>
+  <si>
+    <t>7500 [3900 - 19 000]</t>
+  </si>
+  <si>
+    <t>1700 [1500 - 2000] (Estimates for children are not published because of small numbers.)</t>
+  </si>
+  <si>
+    <t>13 000 [11 000 - 14 000]</t>
+  </si>
+  <si>
+    <t>280 000 [240 000 - 330 000]</t>
+  </si>
+  <si>
+    <t>120 000 [110 000 - 130 000]</t>
+  </si>
+  <si>
+    <t>3300 [2700 - 4100] (Estimates for children are not published because of small numbers.)</t>
+  </si>
+  <si>
+    <t>25 000 [23 000 - 27 000]</t>
+  </si>
+  <si>
+    <t>... [... - ...] (Estimates were unavailable at the time of publication.)</t>
+  </si>
+  <si>
+    <t>9200 [6800 - 12 000]</t>
+  </si>
+  <si>
+    <t>8200 [7400 - 9000] (Historical incidence trends were not available or not reliable.)</t>
+  </si>
+  <si>
+    <t>&lt;500 [&lt;500 - &lt;500] (Estimates are for citizens of the country only. Estimates for children are not published because of small numbers.)</t>
+  </si>
+  <si>
+    <t>12 000 [10 000 - 14 000]</t>
+  </si>
+  <si>
+    <t>2600 [2400 - 2900] (Historical incidence trends were not available or not reliable before 2000. Estimates for children are not published because of small numbers.)</t>
+  </si>
+  <si>
+    <t>19 000 [14 000 - 26 000]</t>
+  </si>
+  <si>
+    <t>4300 [3400 - 5200] (Historical incidence trends were not available or not reliable before 2000.)</t>
+  </si>
+  <si>
+    <t>67 000 [47 000 - 94 000]</t>
+  </si>
+  <si>
+    <t>19 000 [13 000 - 25 000]</t>
+  </si>
+  <si>
+    <t>360 000 [320 000 - 390 000]</t>
+  </si>
+  <si>
+    <t>830 000 [610 000 - 1 100 000]</t>
+  </si>
+  <si>
+    <t>3500 [3100 - 3800] (Historical incidence trends were not available or not reliable. Estimates for children are not published because of small numbers.)</t>
+  </si>
+  <si>
+    <t>95 000 [77 000 - 120 000]</t>
+  </si>
+  <si>
+    <t>84 000 [65 000 - 110 000]</t>
+  </si>
+  <si>
+    <t>2800 [2300 - 3600] (Historical incidence trends were not available or not reliable.)</t>
+  </si>
+  <si>
+    <t>71 000 [62 000 - 82 000]</t>
+  </si>
+  <si>
+    <t>560 000 [470 000 - 650 000]</t>
+  </si>
+  <si>
+    <t>130 000 [110 000 - 160 000]</t>
+  </si>
+  <si>
+    <t>110 000 [94 000 - 130 000]</t>
+  </si>
+  <si>
+    <t>61 000 [55 000 - 68 000]</t>
+  </si>
+  <si>
+    <t>120 000 [100 000 - 150 000]</t>
+  </si>
+  <si>
+    <t>&lt;200 [&lt;100 - &lt;500] (Estimates for children are not published because of small numbers.)</t>
+  </si>
+  <si>
+    <t>91 000 [78 000 - 110 000]</t>
+  </si>
+  <si>
+    <t>13 000 [12 000 - 14 000]</t>
+  </si>
+  <si>
+    <t>1500 [1300 - 1700] (Less than 50 pregnant women in need of PMTCT services.)</t>
+  </si>
+  <si>
+    <t>25 000 [22 000 - 28 000]</t>
+  </si>
+  <si>
+    <t>3400 [3100 - 3600] (Estimates for children are not published because of small numbers.)</t>
+  </si>
+  <si>
+    <t>460 000 [390 000 - 520 000]</t>
+  </si>
+  <si>
+    <t>370 000 [290 000 - 450 000]</t>
+  </si>
+  <si>
+    <t>8600 [5700 - 13 000]</t>
+  </si>
+  <si>
+    <t>67 000 [51 000 - 91 000]</t>
+  </si>
+  <si>
+    <t>33 000 [24 000 - 41 000] (Historical incidence trends were not available or not reliable.)</t>
+  </si>
+  <si>
+    <t>11 000 [10 000 - 12 000]</t>
+  </si>
+  <si>
+    <t>24 000 [22 000 - 26 000]</t>
+  </si>
+  <si>
+    <t>35 000 [28 000 - 45 000]</t>
+  </si>
+  <si>
+    <t>15 000 [10 000 - 21 000]</t>
+  </si>
+  <si>
+    <t>710 000 [570 000 - 880 000]</t>
+  </si>
+  <si>
+    <t>&lt;1000 [&lt;1000 - 1000] (Historical incidence trends were not available or not reliable. Estimates for children are not published because of small numbers.)</t>
+  </si>
+  <si>
+    <t>180 000 [170 000 - 200 000] (Historical incidence trends were not available or not reliable before 2000.)</t>
+  </si>
+  <si>
+    <t>48 000 [38 000 - 59 000]</t>
+  </si>
+  <si>
+    <t>20 000 [17 000 - 24 000]</t>
+  </si>
+  <si>
+    <t>12 000 [8800 - 14 000]</t>
+  </si>
+  <si>
+    <t>290 000 [240 000 - 360 000]</t>
+  </si>
+  <si>
+    <t>46 000 [31 000 - 65 000]</t>
+  </si>
+  <si>
+    <t>36 000 [34 000 - 47 000]</t>
+  </si>
+  <si>
+    <t>8500 [7900 - 9500]</t>
+  </si>
+  <si>
+    <t>150 000 [140 000 - 170 000]</t>
+  </si>
+  <si>
+    <t>21 000 [17 000 - 27 000]</t>
+  </si>
+  <si>
+    <t>2 100 000 [1 700 000 - 2 600 000]</t>
+  </si>
+  <si>
+    <t>620 000 [530 000 - 730 000] (Historical incidence trends were not available or not reliable.)</t>
+  </si>
+  <si>
+    <t>66 000 [37 000 - 120 000]</t>
+  </si>
+  <si>
+    <t>6200 [5700 - 6700] (Historical incidence trends were not available or not reliable before 2000.)</t>
+  </si>
+  <si>
+    <t>130 000 [120 000 - 150 000]</t>
+  </si>
+  <si>
+    <t>30 000 [25 000 - 35 000] (Historical incidence trends were not available or not reliable.)</t>
+  </si>
+  <si>
+    <t>26 000 [22 000 - 30 000]</t>
+  </si>
+  <si>
+    <t>1 600 000 [1 400 000 - 1 800 000]</t>
+  </si>
+  <si>
+    <t>8500 [6300 - 11 000]</t>
+  </si>
+  <si>
+    <t>11 000 [10 000 - 13 000]</t>
+  </si>
+  <si>
+    <t>6600 [5900 - 7400]</t>
+  </si>
+  <si>
+    <t>2200 [2000 - 2600] (Estimates for children are not published because of small numbers.)</t>
+  </si>
+  <si>
+    <t>330 000 [300 000 - 360 000]</t>
+  </si>
+  <si>
+    <t>43 000 [34 000 - 55 000]</t>
+  </si>
+  <si>
+    <t>2900 [2700 - 3300] (Estimates for children are not published because of small numbers.)</t>
+  </si>
+  <si>
+    <t>31 000 [25 000 - 39 000]</t>
+  </si>
+  <si>
+    <t>1 000 000 [970 000 - 1 100 000]</t>
+  </si>
+  <si>
+    <t>97 000 [88 000 - 110 000]</t>
+  </si>
+  <si>
+    <t>110 000 [89 000 - 130 000]</t>
+  </si>
+  <si>
+    <t>&lt;500 [&lt;500 - &lt;500] (Historical incidence trends were not available or not reliable. Estimates for children are not published because of small numbers.)</t>
+  </si>
+  <si>
+    <t>11 000 [7100 - 18 000] (Historical incidence trends were not available or not reliable.)</t>
+  </si>
+  <si>
+    <t>220 000 [200 000 - 240 000]</t>
+  </si>
+  <si>
+    <t>&lt;500 [&lt;500 - &lt;1000] (Estimates for children are not published because of small numbers.)</t>
+  </si>
+  <si>
+    <t>22 000 [16 000 - 28 000]</t>
+  </si>
+  <si>
+    <t>1 800 000 [1 600 000 - 2 100 000]</t>
+  </si>
+  <si>
+    <t>230 000 [200 000 - 260 000]</t>
+  </si>
+  <si>
+    <t>230 000 [210 000 - 260 000]</t>
+  </si>
+  <si>
+    <t>32 000 [28 000 - 38 000]</t>
+  </si>
+  <si>
+    <t>23 000 [20 000 - 26 000]</t>
+  </si>
+  <si>
+    <t>8900 [6800 - 12 000]</t>
+  </si>
+  <si>
+    <t>48 000 [41 000 - 55 000]</t>
+  </si>
+  <si>
+    <t>3 200 000 [2 300 000 - 4 300 000]</t>
+  </si>
+  <si>
+    <t>21 000 [19 000 - 23 000] (Historical incidence trends were not available or not reliable before 2000.)</t>
+  </si>
+  <si>
+    <t>46 000 [40 000 - 51 000]</t>
+  </si>
+  <si>
+    <t>19 000 [12 000 - 39 000]</t>
+  </si>
+  <si>
+    <t>70 000 [55 000 - 94 000] (Historical incidence trends were not available or not reliable.)</t>
+  </si>
+  <si>
+    <t>56 000 [51 000 - 62 000]</t>
+  </si>
+  <si>
+    <t>&lt;100 [&lt;100 - &lt;200] (Estimates are for citizens of the country only. Estimates for children are not published because of small numbers.)</t>
+  </si>
+  <si>
+    <t>15 000 [11 000 - 21 000]</t>
+  </si>
+  <si>
+    <t>16 000 [14 000 - 18 000]</t>
+  </si>
+  <si>
+    <t>220 000 [200 000 - 250 000]</t>
+  </si>
+  <si>
+    <t>8200 [7400 - 9000]</t>
+  </si>
+  <si>
+    <t>41 000 [34 000 - 48 000]</t>
+  </si>
+  <si>
+    <t>2700 [2200 - 3300] (Estimates for children are not published because of small numbers.)</t>
+  </si>
+  <si>
+    <t>67 000 [43 000 - 100 000] (Historical incidence trends were not available or not reliable.)</t>
+  </si>
+  <si>
+    <t>&lt;1000 [&lt;1000 - 1100] (Estimates for children are not published because of small numbers.)</t>
+  </si>
+  <si>
+    <t>24 000 [16 000 - 33 000]</t>
+  </si>
+  <si>
+    <t>7 100 000 [6 400 000 - 7 800 000]</t>
+  </si>
+  <si>
+    <t>200 000 [130 000 - 290 000]</t>
+  </si>
+  <si>
+    <t>140 000 [130 000 - 160 000]</t>
+  </si>
+  <si>
+    <t>4000 [2700 - 6000] (Estimates for children are not published because of small numbers.)</t>
+  </si>
+  <si>
+    <t>56 000 [34 000 - 87 000]</t>
+  </si>
+  <si>
+    <t>4900 [4400 - 5600]</t>
+  </si>
+  <si>
+    <t>220 000 [200 000 - 230 000]</t>
+  </si>
+  <si>
+    <t>14 000 [10 000 - 19 000]</t>
+  </si>
+  <si>
+    <t>450 000 [400 000 - 520 000]</t>
+  </si>
+  <si>
+    <t>&lt;500 [&lt;500 - &lt;500] (Estimates for children are not published because of small numbers.)</t>
+  </si>
+  <si>
+    <t>100 000 [73 000 - 130 000]</t>
+  </si>
+  <si>
+    <t>11 000 [9800 - 12 000]</t>
+  </si>
+  <si>
+    <t>2900 [2000 - 4000] (Estimates for children are not published because of small numbers.)</t>
+  </si>
+  <si>
+    <t>1 400 000 [1 300 000 - 1 500 000]</t>
+  </si>
+  <si>
+    <t>240 000 [220 000 - 260 000]</t>
+  </si>
+  <si>
+    <t>1 400 000 [1 200 000 - 1 600 000]</t>
+  </si>
+  <si>
+    <t>... [... - ...] (Estimates available only through 2008-2014.)</t>
+  </si>
+  <si>
+    <t>12 000 [10 000 - 14 000] (Historical incidence trends were not available or not reliable.)</t>
+  </si>
+  <si>
+    <t>250 000 [220 000 - 290 000]</t>
+  </si>
+  <si>
+    <t>9900 [5600 - 19 000]</t>
+  </si>
+  <si>
+    <t>1 200 000 [1 200 000 - 1 300 000]</t>
+  </si>
+  <si>
+    <t>1 300 000 [1 200 000 - 1 400 000]</t>
+  </si>
+  <si>
+    <t>36 700 000 [30 800 000 - 42 900 000]</t>
   </si>
 </sst>
 </file>
@@ -866,7 +1244,7 @@
   <dimension ref="A1:D170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -892,6 +1270,9 @@
       <c r="B2" t="s">
         <v>3</v>
       </c>
+      <c r="C2" t="s">
+        <v>174</v>
+      </c>
       <c r="D2">
         <v>60.2</v>
       </c>
@@ -903,6 +1284,9 @@
       <c r="B3" t="s">
         <v>4</v>
       </c>
+      <c r="C3" t="s">
+        <v>175</v>
+      </c>
       <c r="D3">
         <v>64.099999999999994</v>
       </c>
@@ -914,6 +1298,9 @@
       <c r="B4" t="s">
         <v>63</v>
       </c>
+      <c r="C4" t="s">
+        <v>176</v>
+      </c>
       <c r="D4">
         <v>51</v>
       </c>
@@ -925,6 +1312,9 @@
       <c r="B5" t="s">
         <v>5</v>
       </c>
+      <c r="C5" t="s">
+        <v>177</v>
+      </c>
       <c r="D5">
         <v>73</v>
       </c>
@@ -936,6 +1326,9 @@
       <c r="B6" t="s">
         <v>64</v>
       </c>
+      <c r="C6" t="s">
+        <v>178</v>
+      </c>
       <c r="D6">
         <v>30.8</v>
       </c>
@@ -947,6 +1340,9 @@
       <c r="B7" t="s">
         <v>6</v>
       </c>
+      <c r="C7" t="s">
+        <v>179</v>
+      </c>
       <c r="D7">
         <v>55.4</v>
       </c>
@@ -958,6 +1354,9 @@
       <c r="B8" t="s">
         <v>65</v>
       </c>
+      <c r="C8" t="s">
+        <v>180</v>
+      </c>
       <c r="D8">
         <v>44.7</v>
       </c>
@@ -969,6 +1368,9 @@
       <c r="B9" t="s">
         <v>66</v>
       </c>
+      <c r="C9" t="s">
+        <v>181</v>
+      </c>
       <c r="D9">
         <v>57.1</v>
       </c>
@@ -980,6 +1382,9 @@
       <c r="B10" t="s">
         <v>67</v>
       </c>
+      <c r="C10" t="s">
+        <v>182</v>
+      </c>
       <c r="D10">
         <v>13.2</v>
       </c>
@@ -991,6 +1396,9 @@
       <c r="B11" t="s">
         <v>68</v>
       </c>
+      <c r="C11" t="s">
+        <v>183</v>
+      </c>
       <c r="D11">
         <v>62.3</v>
       </c>
@@ -1002,6 +1410,9 @@
       <c r="B12" t="s">
         <v>69</v>
       </c>
+      <c r="C12" t="s">
+        <v>184</v>
+      </c>
       <c r="D12">
         <v>25.5</v>
       </c>
@@ -1013,6 +1424,9 @@
       <c r="B13" t="s">
         <v>70</v>
       </c>
+      <c r="C13" t="s">
+        <v>185</v>
+      </c>
       <c r="D13">
         <v>19.399999999999999</v>
       </c>
@@ -1024,6 +1438,9 @@
       <c r="B14" t="s">
         <v>71</v>
       </c>
+      <c r="C14" t="s">
+        <v>186</v>
+      </c>
       <c r="D14">
         <v>40.5</v>
       </c>
@@ -1035,6 +1452,9 @@
       <c r="B15" t="s">
         <v>72</v>
       </c>
+      <c r="C15" t="s">
+        <v>187</v>
+      </c>
       <c r="D15">
         <v>32.6</v>
       </c>
@@ -1046,6 +1466,9 @@
       <c r="B16" t="s">
         <v>73</v>
       </c>
+      <c r="C16" t="s">
+        <v>181</v>
+      </c>
       <c r="D16">
         <v>55.8</v>
       </c>
@@ -1057,6 +1480,9 @@
       <c r="B17" t="s">
         <v>7</v>
       </c>
+      <c r="C17" t="s">
+        <v>188</v>
+      </c>
       <c r="D17">
         <v>35.4</v>
       </c>
@@ -1068,6 +1494,9 @@
       <c r="B18" t="s">
         <v>8</v>
       </c>
+      <c r="C18" t="s">
+        <v>189</v>
+      </c>
       <c r="D18">
         <v>16.399999999999999</v>
       </c>
@@ -1079,6 +1508,9 @@
       <c r="B19" t="s">
         <v>74</v>
       </c>
+      <c r="C19" t="s">
+        <v>181</v>
+      </c>
       <c r="D19">
         <v>44.5</v>
       </c>
@@ -1090,6 +1522,9 @@
       <c r="B20" t="s">
         <v>9</v>
       </c>
+      <c r="C20" t="s">
+        <v>190</v>
+      </c>
       <c r="D20">
         <v>49.2</v>
       </c>
@@ -1101,6 +1536,9 @@
       <c r="B21" t="s">
         <v>10</v>
       </c>
+      <c r="C21" t="s">
+        <v>181</v>
+      </c>
       <c r="D21">
         <v>49.3</v>
       </c>
@@ -1112,6 +1550,9 @@
       <c r="B22" t="s">
         <v>11</v>
       </c>
+      <c r="C22" t="s">
+        <v>191</v>
+      </c>
       <c r="D22">
         <v>59.9</v>
       </c>
@@ -1123,6 +1564,9 @@
       <c r="B23" t="s">
         <v>75</v>
       </c>
+      <c r="C23" t="s">
+        <v>192</v>
+      </c>
       <c r="D23">
         <v>25.3</v>
       </c>
@@ -1134,6 +1578,9 @@
       <c r="B24" t="s">
         <v>76</v>
       </c>
+      <c r="C24" t="s">
+        <v>181</v>
+      </c>
       <c r="D24">
         <v>51</v>
       </c>
@@ -1145,6 +1592,9 @@
       <c r="B25" t="s">
         <v>77</v>
       </c>
+      <c r="C25" t="s">
+        <v>193</v>
+      </c>
       <c r="D25">
         <v>67.7</v>
       </c>
@@ -1156,6 +1606,9 @@
       <c r="B26" t="s">
         <v>12</v>
       </c>
+      <c r="C26" t="s">
+        <v>194</v>
+      </c>
       <c r="D26">
         <v>60.6</v>
       </c>
@@ -1167,6 +1620,9 @@
       <c r="B27" t="s">
         <v>13</v>
       </c>
+      <c r="C27" t="s">
+        <v>195</v>
+      </c>
       <c r="D27">
         <v>80.099999999999994</v>
       </c>
@@ -1178,6 +1634,9 @@
       <c r="B28" t="s">
         <v>78</v>
       </c>
+      <c r="C28" t="s">
+        <v>196</v>
+      </c>
       <c r="D28">
         <v>57.7</v>
       </c>
@@ -1189,6 +1648,9 @@
       <c r="B29" t="s">
         <v>14</v>
       </c>
+      <c r="C29" t="s">
+        <v>197</v>
+      </c>
       <c r="D29">
         <v>44.9</v>
       </c>
@@ -1200,6 +1662,9 @@
       <c r="B30" t="s">
         <v>15</v>
       </c>
+      <c r="C30" t="s">
+        <v>198</v>
+      </c>
       <c r="D30">
         <v>62.8</v>
       </c>
@@ -1211,6 +1676,9 @@
       <c r="B31" t="s">
         <v>79</v>
       </c>
+      <c r="C31" t="s">
+        <v>181</v>
+      </c>
       <c r="D31">
         <v>71</v>
       </c>
@@ -1222,6 +1690,9 @@
       <c r="B32" t="s">
         <v>16</v>
       </c>
+      <c r="C32" t="s">
+        <v>199</v>
+      </c>
       <c r="D32">
         <v>64.8</v>
       </c>
@@ -1233,6 +1704,9 @@
       <c r="B33" t="s">
         <v>80</v>
       </c>
+      <c r="C33" t="s">
+        <v>200</v>
+      </c>
       <c r="D33">
         <v>11.9</v>
       </c>
@@ -1244,6 +1718,9 @@
       <c r="B34" t="s">
         <v>81</v>
       </c>
+      <c r="C34" t="s">
+        <v>201</v>
+      </c>
       <c r="D34">
         <v>57.2</v>
       </c>
@@ -1255,6 +1732,9 @@
       <c r="B35" t="s">
         <v>82</v>
       </c>
+      <c r="C35" t="s">
+        <v>181</v>
+      </c>
       <c r="D35">
         <v>53.5</v>
       </c>
@@ -1266,6 +1746,9 @@
       <c r="B36" t="s">
         <v>83</v>
       </c>
+      <c r="C36" t="s">
+        <v>202</v>
+      </c>
       <c r="D36">
         <v>13.9</v>
       </c>
@@ -1277,6 +1760,9 @@
       <c r="B37" t="s">
         <v>17</v>
       </c>
+      <c r="C37" t="s">
+        <v>203</v>
+      </c>
       <c r="D37">
         <v>52.7</v>
       </c>
@@ -1288,6 +1774,9 @@
       <c r="B38" t="s">
         <v>18</v>
       </c>
+      <c r="C38" t="s">
+        <v>204</v>
+      </c>
       <c r="D38">
         <v>14.9</v>
       </c>
@@ -1299,6 +1788,9 @@
       <c r="B39" t="s">
         <v>84</v>
       </c>
+      <c r="C39" t="s">
+        <v>205</v>
+      </c>
       <c r="D39">
         <v>45.8</v>
       </c>
@@ -1310,6 +1802,9 @@
       <c r="B40" t="s">
         <v>85</v>
       </c>
+      <c r="C40" t="s">
+        <v>206</v>
+      </c>
       <c r="D40">
         <v>75.599999999999994</v>
       </c>
@@ -1321,6 +1816,9 @@
       <c r="B41" t="s">
         <v>19</v>
       </c>
+      <c r="C41" t="s">
+        <v>207</v>
+      </c>
       <c r="D41">
         <v>52</v>
       </c>
@@ -1332,6 +1830,9 @@
       <c r="B42" t="s">
         <v>86</v>
       </c>
+      <c r="C42" t="s">
+        <v>181</v>
+      </c>
       <c r="D42">
         <v>28</v>
       </c>
@@ -1343,6 +1844,9 @@
       <c r="B43" t="s">
         <v>87</v>
       </c>
+      <c r="C43" t="s">
+        <v>208</v>
+      </c>
       <c r="D43">
         <v>13</v>
       </c>
@@ -1354,6 +1858,9 @@
       <c r="B44" t="s">
         <v>20</v>
       </c>
+      <c r="C44" t="s">
+        <v>209</v>
+      </c>
       <c r="D44">
         <v>28.3</v>
       </c>
@@ -1365,6 +1872,9 @@
       <c r="B45" t="s">
         <v>88</v>
       </c>
+      <c r="C45" t="s">
+        <v>181</v>
+      </c>
       <c r="D45">
         <v>71.5</v>
       </c>
@@ -1376,6 +1886,9 @@
       <c r="B46" t="s">
         <v>21</v>
       </c>
+      <c r="C46" t="s">
+        <v>210</v>
+      </c>
       <c r="D46">
         <v>46.8</v>
       </c>
@@ -1387,6 +1900,9 @@
       <c r="B47" t="s">
         <v>89</v>
       </c>
+      <c r="C47" t="s">
+        <v>181</v>
+      </c>
       <c r="D47">
         <v>49</v>
       </c>
@@ -1398,6 +1914,9 @@
       <c r="B48" t="s">
         <v>90</v>
       </c>
+      <c r="C48" t="s">
+        <v>211</v>
+      </c>
       <c r="D48">
         <v>70.8</v>
       </c>
@@ -1409,6 +1928,9 @@
       <c r="B49" t="s">
         <v>22</v>
       </c>
+      <c r="C49" t="s">
+        <v>212</v>
+      </c>
       <c r="D49">
         <v>9.9</v>
       </c>
@@ -1420,6 +1942,9 @@
       <c r="B50" t="s">
         <v>91</v>
       </c>
+      <c r="C50" t="s">
+        <v>213</v>
+      </c>
       <c r="D50">
         <v>84.2</v>
       </c>
@@ -1431,6 +1956,9 @@
       <c r="B51" t="s">
         <v>92</v>
       </c>
+      <c r="C51" t="s">
+        <v>214</v>
+      </c>
       <c r="D51">
         <v>51.7</v>
       </c>
@@ -1442,6 +1970,9 @@
       <c r="B52" t="s">
         <v>93</v>
       </c>
+      <c r="C52" t="s">
+        <v>215</v>
+      </c>
       <c r="D52">
         <v>53.4</v>
       </c>
@@ -1453,6 +1984,9 @@
       <c r="B53" t="s">
         <v>94</v>
       </c>
+      <c r="C53" t="s">
+        <v>216</v>
+      </c>
       <c r="D53">
         <v>12.5</v>
       </c>
@@ -1464,6 +1998,9 @@
       <c r="B54" t="s">
         <v>95</v>
       </c>
+      <c r="C54" t="s">
+        <v>217</v>
+      </c>
       <c r="D54">
         <v>63.2</v>
       </c>
@@ -1475,6 +2012,9 @@
       <c r="B55" t="s">
         <v>96</v>
       </c>
+      <c r="C55" t="s">
+        <v>181</v>
+      </c>
       <c r="D55">
         <v>45.8</v>
       </c>
@@ -1486,6 +2026,9 @@
       <c r="B56" t="s">
         <v>23</v>
       </c>
+      <c r="C56" t="s">
+        <v>218</v>
+      </c>
       <c r="D56">
         <v>26.2</v>
       </c>
@@ -1497,6 +2040,9 @@
       <c r="B57" t="s">
         <v>97</v>
       </c>
+      <c r="C57" t="s">
+        <v>219</v>
+      </c>
       <c r="D57">
         <v>65.099999999999994</v>
       </c>
@@ -1508,6 +2054,9 @@
       <c r="B58" t="s">
         <v>98</v>
       </c>
+      <c r="C58" t="s">
+        <v>181</v>
+      </c>
       <c r="D58">
         <v>26.8</v>
       </c>
@@ -1519,6 +2068,9 @@
       <c r="B59" t="s">
         <v>99</v>
       </c>
+      <c r="C59" t="s">
+        <v>220</v>
+      </c>
       <c r="D59">
         <v>18</v>
       </c>
@@ -1530,6 +2082,9 @@
       <c r="B60" t="s">
         <v>24</v>
       </c>
+      <c r="C60" t="s">
+        <v>221</v>
+      </c>
       <c r="D60">
         <v>17.8</v>
       </c>
@@ -1538,550 +2093,880 @@
       <c r="B61" t="s">
         <v>25</v>
       </c>
+      <c r="C61" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
         <v>100</v>
       </c>
+      <c r="C62" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
         <v>101</v>
       </c>
+      <c r="C63" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C64" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C65" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C66" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C67" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C68" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C69" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C70" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C71" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C72" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C73" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C74" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C75" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C76" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C77" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C78" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C79" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C80" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C81" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C82" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C83" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C84" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B85" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C85" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B86" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C86" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C87" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="88" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B88" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C88" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="89" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C89" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="90" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B90" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C90" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="91" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C91" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="92" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C92" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="93" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C93" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="94" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B94" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C94" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="95" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B95" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C95" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="96" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B96" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C96" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="97" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B97" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C97" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="98" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B98" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C98" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="99" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B99" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C99" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="100" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B100" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C100" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="101" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B101" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C101" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="102" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B102" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C102" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="103" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B103" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C103" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="104" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B104" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C104" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="105" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B105" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C105" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="106" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B106" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C106" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="107" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B107" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C107" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="108" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B108" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C108" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="109" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B109" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C109" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="110" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B110" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C110" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="111" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B111" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C111" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="112" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B112" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C112" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="113" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B113" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C113" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="114" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B114" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C114" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="115" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B115" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C115" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="116" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B116" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C116" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="117" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B117" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C117" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="118" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B118" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C118" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="119" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B119" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C119" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="120" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B120" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C120" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="121" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B121" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C121" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="122" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B122" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C122" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="123" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B123" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C123" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="124" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B124" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C124" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="125" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B125" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C125" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="126" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B126" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C126" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="127" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B127" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C127" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="128" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B128" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C128" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="129" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B129" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C129" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="130" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B130" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C130" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="131" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B131" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C131" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="132" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B132" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C132" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="133" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B133" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C133" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="134" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B134" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C134" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="135" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B135" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C135" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="136" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B136" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C136" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="137" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B137" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C137" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="138" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B138" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C138" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="139" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B139" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C139" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="140" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B140" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C140" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="141" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B141" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C141" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="142" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B142" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="143" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C142" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="143" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B143" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="144" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C143" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="144" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B144" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C144" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="145" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B145" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C145" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="146" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B146" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="147" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C146" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="147" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B147" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="148" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C147" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="148" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B148" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="149" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C148" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="149" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B149" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C149" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="150" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B150" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="151" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C150" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="151" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B151" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="152" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C151" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="152" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B152" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="153" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C152" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="153" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B153" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="154" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C153" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="154" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B154" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="155" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C154" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="155" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B155" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="156" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C155" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="156" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B156" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="157" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C156" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="157" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B157" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="158" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C157" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="158" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B158" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="159" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C158" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="159" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B159" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="160" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C159" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="160" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B160" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="161" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C160" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="161" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B161" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="162" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C161" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="162" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B162" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="163" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C162" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="163" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B163" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="164" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C163" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="164" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B164" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="165" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C164" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="165" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B165" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="166" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C165" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="166" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B166" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="167" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C166" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="167" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B167" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="168" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C167" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="168" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B168" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="169" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C168" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="169" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B169" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="170" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C169" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="170" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B170" t="s">
         <v>173</v>
+      </c>
+      <c r="C170" t="s">
+        <v>299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed records where Country = ‘Timor-Leste’ and ‘Bosnia and Herzegovina’ because population data was not recorded (delete, 2x).
</commit_message>
<xml_diff>
--- a/GlobalHIVMerged.xlsx
+++ b/GlobalHIVMerged.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="118">
   <si>
     <t>Country</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Bolivia (Plurinational State of)</t>
   </si>
   <si>
-    <t>Bosnia and Herzegovina</t>
-  </si>
-  <si>
     <t>Botswana</t>
   </si>
   <si>
@@ -194,9 +191,6 @@
     <t>Swaziland</t>
   </si>
   <si>
-    <t>Timor-Leste</t>
-  </si>
-  <si>
     <t>Togo</t>
   </si>
   <si>
@@ -231,9 +225,6 @@
   </si>
   <si>
     <t>3300 [2700 - 4100] (Estimates for children are not published because of small numbers.)</t>
-  </si>
-  <si>
-    <t>... [... - ...] (Estimates were unavailable at the time of publication.)</t>
   </si>
   <si>
     <t>4300 [3400 - 5200] (Historical incidence trends were not available or not reliable before 2000.)</t>
@@ -704,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:D58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -717,7 +708,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -734,7 +725,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D2">
         <v>60.2</v>
@@ -748,7 +739,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D3">
         <v>64.099999999999994</v>
@@ -762,7 +753,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D4">
         <v>51</v>
@@ -776,7 +767,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D5">
         <v>73</v>
@@ -790,7 +781,7 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D6">
         <v>30.8</v>
@@ -804,7 +795,7 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D7">
         <v>55.4</v>
@@ -818,7 +809,7 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D8">
         <v>44.7</v>
@@ -832,10 +823,10 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D9">
-        <v>57.1</v>
+        <v>13.2</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -846,10 +837,10 @@
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D10">
-        <v>13.2</v>
+        <v>62.3</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -860,10 +851,10 @@
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D11">
-        <v>62.3</v>
+        <v>25.5</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -874,10 +865,10 @@
         <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D12">
-        <v>25.5</v>
+        <v>19.399999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -888,10 +879,10 @@
         <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D13">
-        <v>19.399999999999999</v>
+        <v>40.5</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -902,10 +893,10 @@
         <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D14">
-        <v>40.5</v>
+        <v>32.6</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -916,10 +907,10 @@
         <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D15">
-        <v>32.6</v>
+        <v>55.8</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -930,10 +921,10 @@
         <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D16">
-        <v>55.8</v>
+        <v>35.4</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -944,10 +935,10 @@
         <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>80</v>
+        <v>117</v>
       </c>
       <c r="D17">
-        <v>35.4</v>
+        <v>16.399999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -958,10 +949,10 @@
         <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>120</v>
+        <v>78</v>
       </c>
       <c r="D18">
-        <v>16.399999999999999</v>
+        <v>44.5</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -972,10 +963,10 @@
         <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D19">
-        <v>44.5</v>
+        <v>49.2</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -986,10 +977,10 @@
         <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D20">
-        <v>49.2</v>
+        <v>49.3</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -1000,10 +991,10 @@
         <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D21">
-        <v>49.3</v>
+        <v>59.9</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -1014,10 +1005,10 @@
         <v>23</v>
       </c>
       <c r="C22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D22">
-        <v>59.9</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -1028,10 +1019,10 @@
         <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D23">
-        <v>25.3</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -1042,10 +1033,10 @@
         <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D24">
-        <v>51</v>
+        <v>67.7</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -1056,10 +1047,10 @@
         <v>26</v>
       </c>
       <c r="C25" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D25">
-        <v>67.7</v>
+        <v>60.6</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -1070,10 +1061,10 @@
         <v>27</v>
       </c>
       <c r="C26" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="D26">
-        <v>60.6</v>
+        <v>80.099999999999994</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -1084,10 +1075,10 @@
         <v>28</v>
       </c>
       <c r="C27" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="D27">
-        <v>80.099999999999994</v>
+        <v>57.7</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -1098,10 +1089,10 @@
         <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D28">
-        <v>57.7</v>
+        <v>44.9</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -1112,10 +1103,10 @@
         <v>30</v>
       </c>
       <c r="C29" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D29">
-        <v>44.9</v>
+        <v>62.8</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -1126,10 +1117,10 @@
         <v>31</v>
       </c>
       <c r="C30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D30">
-        <v>62.8</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -1140,10 +1131,10 @@
         <v>32</v>
       </c>
       <c r="C31" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D31">
-        <v>71</v>
+        <v>64.8</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -1154,10 +1145,10 @@
         <v>33</v>
       </c>
       <c r="C32" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D32">
-        <v>64.8</v>
+        <v>11.9</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -1168,10 +1159,10 @@
         <v>34</v>
       </c>
       <c r="C33" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D33">
-        <v>11.9</v>
+        <v>57.2</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -1182,10 +1173,10 @@
         <v>35</v>
       </c>
       <c r="C34" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D34">
-        <v>57.2</v>
+        <v>53.5</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -1196,10 +1187,10 @@
         <v>36</v>
       </c>
       <c r="C35" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D35">
-        <v>53.5</v>
+        <v>13.9</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -1210,10 +1201,10 @@
         <v>37</v>
       </c>
       <c r="C36" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D36">
-        <v>13.9</v>
+        <v>52.7</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -1224,10 +1215,10 @@
         <v>38</v>
       </c>
       <c r="C37" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D37">
-        <v>52.7</v>
+        <v>14.9</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -1238,10 +1229,10 @@
         <v>39</v>
       </c>
       <c r="C38" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D38">
-        <v>14.9</v>
+        <v>45.8</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -1252,10 +1243,10 @@
         <v>40</v>
       </c>
       <c r="C39" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D39">
-        <v>45.8</v>
+        <v>75.599999999999994</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -1266,10 +1257,10 @@
         <v>41</v>
       </c>
       <c r="C40" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D40">
-        <v>75.599999999999994</v>
+        <v>52</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -1280,10 +1271,10 @@
         <v>42</v>
       </c>
       <c r="C41" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D41">
-        <v>52</v>
+        <v>28</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -1294,10 +1285,10 @@
         <v>43</v>
       </c>
       <c r="C42" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D42">
-        <v>28</v>
+        <v>13</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -1308,10 +1299,10 @@
         <v>44</v>
       </c>
       <c r="C43" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D43">
-        <v>13</v>
+        <v>28.3</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -1322,10 +1313,10 @@
         <v>45</v>
       </c>
       <c r="C44" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D44">
-        <v>28.3</v>
+        <v>71.5</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -1336,10 +1327,10 @@
         <v>46</v>
       </c>
       <c r="C45" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D45">
-        <v>71.5</v>
+        <v>46.8</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -1350,10 +1341,10 @@
         <v>47</v>
       </c>
       <c r="C46" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="D46">
-        <v>46.8</v>
+        <v>49</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -1364,10 +1355,10 @@
         <v>48</v>
       </c>
       <c r="C47" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="D47">
-        <v>49</v>
+        <v>70.8</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -1378,10 +1369,10 @@
         <v>49</v>
       </c>
       <c r="C48" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D48">
-        <v>70.8</v>
+        <v>9.9</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -1389,13 +1380,13 @@
         <v>50</v>
       </c>
       <c r="B49" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C49" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D49">
-        <v>9.9</v>
+        <v>84.2</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -1403,13 +1394,13 @@
         <v>51</v>
       </c>
       <c r="B50" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="C50" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D50">
-        <v>84.2</v>
+        <v>51.7</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -1420,10 +1411,10 @@
         <v>52</v>
       </c>
       <c r="C51" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D51">
-        <v>51.7</v>
+        <v>53.4</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
@@ -1434,10 +1425,10 @@
         <v>53</v>
       </c>
       <c r="C52" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D52">
-        <v>53.4</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -1448,10 +1439,10 @@
         <v>54</v>
       </c>
       <c r="C53" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D53">
-        <v>12.5</v>
+        <v>45.8</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -1462,10 +1453,10 @@
         <v>55</v>
       </c>
       <c r="C54" t="s">
-        <v>68</v>
+        <v>112</v>
       </c>
       <c r="D54">
-        <v>63.2</v>
+        <v>26.2</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -1476,10 +1467,10 @@
         <v>56</v>
       </c>
       <c r="C55" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D55">
-        <v>45.8</v>
+        <v>65.099999999999994</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -1490,10 +1481,10 @@
         <v>57</v>
       </c>
       <c r="C56" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D56">
-        <v>26.2</v>
+        <v>26.8</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -1504,10 +1495,10 @@
         <v>58</v>
       </c>
       <c r="C57" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D57">
-        <v>65.099999999999994</v>
+        <v>18</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -1518,37 +1509,9 @@
         <v>59</v>
       </c>
       <c r="C58" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D58">
-        <v>26.8</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>60</v>
-      </c>
-      <c r="B59" t="s">
-        <v>60</v>
-      </c>
-      <c r="C59" t="s">
-        <v>118</v>
-      </c>
-      <c r="D59">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>61</v>
-      </c>
-      <c r="B60" t="s">
-        <v>61</v>
-      </c>
-      <c r="C60" t="s">
-        <v>119</v>
-      </c>
-      <c r="D60">
         <v>17.8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed parenthetical info from ‘Number of People Living with HIV’ by using find and replace with regexp ‘]*’ (1 operations, 59 records affected).
</commit_message>
<xml_diff>
--- a/GlobalHIVMerged.xlsx
+++ b/GlobalHIVMerged.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="106">
   <si>
     <t>Country</t>
   </si>
@@ -215,172 +215,136 @@
     <t>Saudi Arabia</t>
   </si>
   <si>
-    <t>7500 [3900 - 19 000]</t>
-  </si>
-  <si>
-    <t>1700 [1500 - 2000] (Estimates for children are not published because of small numbers.)</t>
-  </si>
-  <si>
-    <t>280 000 [240 000 - 330 000]</t>
-  </si>
-  <si>
-    <t>3300 [2700 - 4100] (Estimates for children are not published because of small numbers.)</t>
-  </si>
-  <si>
-    <t>4300 [3400 - 5200] (Historical incidence trends were not available or not reliable before 2000.)</t>
-  </si>
-  <si>
-    <t>67 000 [47 000 - 94 000]</t>
-  </si>
-  <si>
-    <t>19 000 [13 000 - 25 000]</t>
-  </si>
-  <si>
-    <t>360 000 [320 000 - 390 000]</t>
-  </si>
-  <si>
-    <t>95 000 [77 000 - 120 000]</t>
-  </si>
-  <si>
-    <t>84 000 [65 000 - 110 000]</t>
-  </si>
-  <si>
-    <t>71 000 [62 000 - 82 000]</t>
-  </si>
-  <si>
-    <t>560 000 [470 000 - 650 000]</t>
-  </si>
-  <si>
-    <t>130 000 [110 000 - 160 000]</t>
-  </si>
-  <si>
-    <t>120 000 [100 000 - 150 000]</t>
-  </si>
-  <si>
-    <t>&lt;200 [&lt;100 - &lt;500] (Estimates for children are not published because of small numbers.)</t>
-  </si>
-  <si>
-    <t>91 000 [78 000 - 110 000]</t>
-  </si>
-  <si>
-    <t>460 000 [390 000 - 520 000]</t>
-  </si>
-  <si>
-    <t>370 000 [290 000 - 450 000]</t>
-  </si>
-  <si>
-    <t>67 000 [51 000 - 91 000]</t>
-  </si>
-  <si>
-    <t>710 000 [570 000 - 880 000]</t>
-  </si>
-  <si>
-    <t>48 000 [38 000 - 59 000]</t>
-  </si>
-  <si>
-    <t>20 000 [17 000 - 24 000]</t>
-  </si>
-  <si>
-    <t>290 000 [240 000 - 360 000]</t>
-  </si>
-  <si>
-    <t>46 000 [31 000 - 65 000]</t>
-  </si>
-  <si>
-    <t>150 000 [140 000 - 170 000]</t>
-  </si>
-  <si>
-    <t>21 000 [17 000 - 27 000]</t>
-  </si>
-  <si>
-    <t>620 000 [530 000 - 730 000] (Historical incidence trends were not available or not reliable.)</t>
-  </si>
-  <si>
-    <t>130 000 [120 000 - 150 000]</t>
-  </si>
-  <si>
-    <t>30 000 [25 000 - 35 000] (Historical incidence trends were not available or not reliable.)</t>
-  </si>
-  <si>
-    <t>26 000 [22 000 - 30 000]</t>
-  </si>
-  <si>
-    <t>1 600 000 [1 400 000 - 1 800 000]</t>
-  </si>
-  <si>
-    <t>8500 [6300 - 11 000]</t>
-  </si>
-  <si>
-    <t>11 000 [10 000 - 13 000]</t>
-  </si>
-  <si>
-    <t>330 000 [300 000 - 360 000]</t>
-  </si>
-  <si>
-    <t>43 000 [34 000 - 55 000]</t>
-  </si>
-  <si>
-    <t>1 000 000 [970 000 - 1 100 000]</t>
-  </si>
-  <si>
-    <t>110 000 [89 000 - 130 000]</t>
-  </si>
-  <si>
-    <t>&lt;500 [&lt;500 - &lt;1000] (Estimates for children are not published because of small numbers.)</t>
-  </si>
-  <si>
-    <t>1 800 000 [1 600 000 - 2 100 000]</t>
-  </si>
-  <si>
-    <t>230 000 [210 000 - 260 000]</t>
-  </si>
-  <si>
-    <t>32 000 [28 000 - 38 000]</t>
-  </si>
-  <si>
-    <t>48 000 [41 000 - 55 000]</t>
-  </si>
-  <si>
-    <t>3 200 000 [2 300 000 - 4 300 000]</t>
-  </si>
-  <si>
-    <t>15 000 [11 000 - 21 000]</t>
-  </si>
-  <si>
-    <t>220 000 [200 000 - 250 000]</t>
-  </si>
-  <si>
-    <t>8200 [7400 - 9000]</t>
-  </si>
-  <si>
-    <t>41 000 [34 000 - 48 000]</t>
-  </si>
-  <si>
-    <t>67 000 [43 000 - 100 000] (Historical incidence trends were not available or not reliable.)</t>
-  </si>
-  <si>
-    <t>220 000 [200 000 - 230 000]</t>
-  </si>
-  <si>
-    <t>100 000 [73 000 - 130 000]</t>
-  </si>
-  <si>
-    <t>1 400 000 [1 300 000 - 1 500 000]</t>
-  </si>
-  <si>
-    <t>240 000 [220 000 - 260 000]</t>
-  </si>
-  <si>
-    <t>1 400 000 [1 200 000 - 1 600 000]</t>
-  </si>
-  <si>
-    <t>1 200 000 [1 200 000 - 1 300 000]</t>
-  </si>
-  <si>
-    <t>1 300 000 [1 200 000 - 1 400 000]</t>
-  </si>
-  <si>
-    <t>25 000 [22 000 - 28 000]</t>
+    <t xml:space="preserve">280 000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">67 000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">19 000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">360 000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">95 000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">84 000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">71 000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">560 000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">130 000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;200 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">91 000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">25 000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">460 000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">370 000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">710 000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">48 000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">290 000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">46 000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">120 000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">150 000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">21 000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">620 000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">26 000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 600 000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">330 000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">43 000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 000 000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">110 000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;500 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 800 000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">230 000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">32 000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 200 000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">220 000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">41 000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">100 000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 400 000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">240 000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 200 000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 300 000 </t>
   </si>
 </sst>
 </file>
@@ -698,7 +662,7 @@
   <dimension ref="A1:D58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -724,8 +688,8 @@
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>62</v>
+      <c r="C2">
+        <v>7500</v>
       </c>
       <c r="D2">
         <v>60.2</v>
@@ -738,8 +702,8 @@
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
-        <v>63</v>
+      <c r="C3">
+        <v>1700</v>
       </c>
       <c r="D3">
         <v>64.099999999999994</v>
@@ -753,7 +717,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D4">
         <v>51</v>
@@ -766,8 +730,8 @@
       <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
-        <v>65</v>
+      <c r="C5">
+        <v>3300</v>
       </c>
       <c r="D5">
         <v>73</v>
@@ -780,8 +744,8 @@
       <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" t="s">
-        <v>66</v>
+      <c r="C6">
+        <v>4300</v>
       </c>
       <c r="D6">
         <v>30.8</v>
@@ -795,7 +759,7 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D7">
         <v>55.4</v>
@@ -809,7 +773,7 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D8">
         <v>44.7</v>
@@ -823,7 +787,7 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D9">
         <v>13.2</v>
@@ -837,7 +801,7 @@
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D10">
         <v>62.3</v>
@@ -851,7 +815,7 @@
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D11">
         <v>25.5</v>
@@ -865,7 +829,7 @@
         <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D12">
         <v>19.399999999999999</v>
@@ -879,7 +843,7 @@
         <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D13">
         <v>40.5</v>
@@ -893,7 +857,7 @@
         <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D14">
         <v>32.6</v>
@@ -907,7 +871,7 @@
         <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D15">
         <v>55.8</v>
@@ -921,7 +885,7 @@
         <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D16">
         <v>35.4</v>
@@ -935,7 +899,7 @@
         <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>117</v>
+        <v>73</v>
       </c>
       <c r="D17">
         <v>16.399999999999999</v>
@@ -949,7 +913,7 @@
         <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D18">
         <v>44.5</v>
@@ -963,7 +927,7 @@
         <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D19">
         <v>49.2</v>
@@ -977,7 +941,7 @@
         <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="D20">
         <v>49.3</v>
@@ -991,7 +955,7 @@
         <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D21">
         <v>59.9</v>
@@ -1005,7 +969,7 @@
         <v>23</v>
       </c>
       <c r="C22" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D22">
         <v>25.3</v>
@@ -1019,7 +983,7 @@
         <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D23">
         <v>51</v>
@@ -1033,7 +997,7 @@
         <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D24">
         <v>67.7</v>
@@ -1047,7 +1011,7 @@
         <v>26</v>
       </c>
       <c r="C25" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D25">
         <v>60.6</v>
@@ -1061,7 +1025,7 @@
         <v>27</v>
       </c>
       <c r="C26" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="D26">
         <v>80.099999999999994</v>
@@ -1075,7 +1039,7 @@
         <v>28</v>
       </c>
       <c r="C27" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D27">
         <v>57.7</v>
@@ -1089,7 +1053,7 @@
         <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D28">
         <v>44.9</v>
@@ -1103,7 +1067,7 @@
         <v>30</v>
       </c>
       <c r="C29" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D29">
         <v>62.8</v>
@@ -1117,7 +1081,7 @@
         <v>31</v>
       </c>
       <c r="C30" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D30">
         <v>71</v>
@@ -1131,7 +1095,7 @@
         <v>32</v>
       </c>
       <c r="C31" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D31">
         <v>64.8</v>
@@ -1145,7 +1109,7 @@
         <v>33</v>
       </c>
       <c r="C32" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D32">
         <v>11.9</v>
@@ -1158,8 +1122,8 @@
       <c r="B33" t="s">
         <v>34</v>
       </c>
-      <c r="C33" t="s">
-        <v>93</v>
+      <c r="C33">
+        <v>8500</v>
       </c>
       <c r="D33">
         <v>57.2</v>
@@ -1173,7 +1137,7 @@
         <v>35</v>
       </c>
       <c r="C34" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D34">
         <v>53.5</v>
@@ -1187,7 +1151,7 @@
         <v>36</v>
       </c>
       <c r="C35" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D35">
         <v>13.9</v>
@@ -1201,7 +1165,7 @@
         <v>37</v>
       </c>
       <c r="C36" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D36">
         <v>52.7</v>
@@ -1215,7 +1179,7 @@
         <v>38</v>
       </c>
       <c r="C37" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D37">
         <v>14.9</v>
@@ -1229,7 +1193,7 @@
         <v>39</v>
       </c>
       <c r="C38" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D38">
         <v>45.8</v>
@@ -1243,7 +1207,7 @@
         <v>40</v>
       </c>
       <c r="C39" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D39">
         <v>75.599999999999994</v>
@@ -1257,7 +1221,7 @@
         <v>41</v>
       </c>
       <c r="C40" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D40">
         <v>52</v>
@@ -1271,7 +1235,7 @@
         <v>42</v>
       </c>
       <c r="C41" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D41">
         <v>28</v>
@@ -1285,7 +1249,7 @@
         <v>43</v>
       </c>
       <c r="C42" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D42">
         <v>13</v>
@@ -1299,7 +1263,7 @@
         <v>44</v>
       </c>
       <c r="C43" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D43">
         <v>28.3</v>
@@ -1313,7 +1277,7 @@
         <v>45</v>
       </c>
       <c r="C44" t="s">
-        <v>103</v>
+        <v>77</v>
       </c>
       <c r="D44">
         <v>71.5</v>
@@ -1327,7 +1291,7 @@
         <v>46</v>
       </c>
       <c r="C45" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="D45">
         <v>46.8</v>
@@ -1341,7 +1305,7 @@
         <v>47</v>
       </c>
       <c r="C46" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="D46">
         <v>49</v>
@@ -1355,7 +1319,7 @@
         <v>48</v>
       </c>
       <c r="C47" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D47">
         <v>70.8</v>
@@ -1369,7 +1333,7 @@
         <v>49</v>
       </c>
       <c r="C48" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D48">
         <v>9.9</v>
@@ -1382,8 +1346,8 @@
       <c r="B49" t="s">
         <v>61</v>
       </c>
-      <c r="C49" t="s">
-        <v>107</v>
+      <c r="C49">
+        <v>8200</v>
       </c>
       <c r="D49">
         <v>84.2</v>
@@ -1397,7 +1361,7 @@
         <v>51</v>
       </c>
       <c r="C50" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D50">
         <v>51.7</v>
@@ -1411,7 +1375,7 @@
         <v>52</v>
       </c>
       <c r="C51" t="s">
-        <v>109</v>
+        <v>63</v>
       </c>
       <c r="D51">
         <v>53.4</v>
@@ -1425,7 +1389,7 @@
         <v>53</v>
       </c>
       <c r="C52" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="D52">
         <v>12.5</v>
@@ -1439,7 +1403,7 @@
         <v>54</v>
       </c>
       <c r="C53" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="D53">
         <v>45.8</v>
@@ -1453,7 +1417,7 @@
         <v>55</v>
       </c>
       <c r="C54" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="D54">
         <v>26.2</v>
@@ -1467,7 +1431,7 @@
         <v>56</v>
       </c>
       <c r="C55" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="D55">
         <v>65.099999999999994</v>
@@ -1481,7 +1445,7 @@
         <v>57</v>
       </c>
       <c r="C56" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="D56">
         <v>26.8</v>
@@ -1495,7 +1459,7 @@
         <v>58</v>
       </c>
       <c r="C57" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="D57">
         <v>18</v>
@@ -1509,7 +1473,7 @@
         <v>59</v>
       </c>
       <c r="C58" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="D58">
         <v>17.8</v>

</xml_diff>

<commit_message>
Removed spaces from ‘Number of People Living with HIV’ by using find and replace with regexp ‘ ’ (1 operation, 59 records affected).
</commit_message>
<xml_diff>
--- a/GlobalHIVMerged.xlsx
+++ b/GlobalHIVMerged.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="64">
   <si>
     <t>Country</t>
   </si>
@@ -215,136 +215,10 @@
     <t>Saudi Arabia</t>
   </si>
   <si>
-    <t xml:space="preserve">280 000 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">67 000 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">19 000 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">360 000 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">95 000 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">84 000 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">71 000 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">560 000 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">130 000 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;200 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">91 000 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">25 000 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">460 000 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">370 000 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">710 000 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">48 000 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">20 000 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">290 000 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">46 000 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">120 000 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">150 000 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">21 000 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">620 000 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">30 000 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">26 000 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 600 000 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">11 000 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">330 000 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">43 000 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 000 000 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">110 000 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;500 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 800 000 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">230 000 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">32 000 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 200 000 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">15 000 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">220 000 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">41 000 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">100 000 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 400 000 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">240 000 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 200 000 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 300 000 </t>
+    <t>&lt;200</t>
+  </si>
+  <si>
+    <t>&lt;500</t>
   </si>
 </sst>
 </file>
@@ -661,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -716,8 +590,8 @@
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
-        <v>62</v>
+      <c r="C4">
+        <v>280000</v>
       </c>
       <c r="D4">
         <v>51</v>
@@ -758,8 +632,8 @@
       <c r="B7" t="s">
         <v>8</v>
       </c>
-      <c r="C7" t="s">
-        <v>63</v>
+      <c r="C7">
+        <v>67000</v>
       </c>
       <c r="D7">
         <v>55.4</v>
@@ -772,8 +646,8 @@
       <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="C8" t="s">
-        <v>64</v>
+      <c r="C8">
+        <v>19000</v>
       </c>
       <c r="D8">
         <v>44.7</v>
@@ -786,8 +660,8 @@
       <c r="B9" t="s">
         <v>10</v>
       </c>
-      <c r="C9" t="s">
-        <v>65</v>
+      <c r="C9">
+        <v>360000</v>
       </c>
       <c r="D9">
         <v>13.2</v>
@@ -800,8 +674,8 @@
       <c r="B10" t="s">
         <v>11</v>
       </c>
-      <c r="C10" t="s">
-        <v>66</v>
+      <c r="C10">
+        <v>95000</v>
       </c>
       <c r="D10">
         <v>62.3</v>
@@ -814,8 +688,8 @@
       <c r="B11" t="s">
         <v>12</v>
       </c>
-      <c r="C11" t="s">
-        <v>67</v>
+      <c r="C11">
+        <v>84000</v>
       </c>
       <c r="D11">
         <v>25.5</v>
@@ -828,8 +702,8 @@
       <c r="B12" t="s">
         <v>13</v>
       </c>
-      <c r="C12" t="s">
-        <v>68</v>
+      <c r="C12">
+        <v>71000</v>
       </c>
       <c r="D12">
         <v>19.399999999999999</v>
@@ -842,8 +716,8 @@
       <c r="B13" t="s">
         <v>14</v>
       </c>
-      <c r="C13" t="s">
-        <v>69</v>
+      <c r="C13">
+        <v>560000</v>
       </c>
       <c r="D13">
         <v>40.5</v>
@@ -856,8 +730,8 @@
       <c r="B14" t="s">
         <v>15</v>
       </c>
-      <c r="C14" t="s">
-        <v>70</v>
+      <c r="C14">
+        <v>130000</v>
       </c>
       <c r="D14">
         <v>32.6</v>
@@ -871,7 +745,7 @@
         <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="D15">
         <v>55.8</v>
@@ -884,8 +758,8 @@
       <c r="B16" t="s">
         <v>17</v>
       </c>
-      <c r="C16" t="s">
-        <v>72</v>
+      <c r="C16">
+        <v>91000</v>
       </c>
       <c r="D16">
         <v>35.4</v>
@@ -898,8 +772,8 @@
       <c r="B17" t="s">
         <v>18</v>
       </c>
-      <c r="C17" t="s">
-        <v>73</v>
+      <c r="C17">
+        <v>25000</v>
       </c>
       <c r="D17">
         <v>16.399999999999999</v>
@@ -912,8 +786,8 @@
       <c r="B18" t="s">
         <v>19</v>
       </c>
-      <c r="C18" t="s">
-        <v>74</v>
+      <c r="C18">
+        <v>460000</v>
       </c>
       <c r="D18">
         <v>44.5</v>
@@ -926,8 +800,8 @@
       <c r="B19" t="s">
         <v>20</v>
       </c>
-      <c r="C19" t="s">
-        <v>75</v>
+      <c r="C19">
+        <v>370000</v>
       </c>
       <c r="D19">
         <v>49.2</v>
@@ -940,8 +814,8 @@
       <c r="B20" t="s">
         <v>21</v>
       </c>
-      <c r="C20" t="s">
-        <v>63</v>
+      <c r="C20">
+        <v>67000</v>
       </c>
       <c r="D20">
         <v>49.3</v>
@@ -954,8 +828,8 @@
       <c r="B21" t="s">
         <v>22</v>
       </c>
-      <c r="C21" t="s">
-        <v>76</v>
+      <c r="C21">
+        <v>710000</v>
       </c>
       <c r="D21">
         <v>59.9</v>
@@ -968,8 +842,8 @@
       <c r="B22" t="s">
         <v>23</v>
       </c>
-      <c r="C22" t="s">
-        <v>77</v>
+      <c r="C22">
+        <v>48000</v>
       </c>
       <c r="D22">
         <v>25.3</v>
@@ -982,8 +856,8 @@
       <c r="B23" t="s">
         <v>24</v>
       </c>
-      <c r="C23" t="s">
-        <v>78</v>
+      <c r="C23">
+        <v>20000</v>
       </c>
       <c r="D23">
         <v>51</v>
@@ -996,8 +870,8 @@
       <c r="B24" t="s">
         <v>25</v>
       </c>
-      <c r="C24" t="s">
-        <v>79</v>
+      <c r="C24">
+        <v>290000</v>
       </c>
       <c r="D24">
         <v>67.7</v>
@@ -1010,8 +884,8 @@
       <c r="B25" t="s">
         <v>26</v>
       </c>
-      <c r="C25" t="s">
-        <v>80</v>
+      <c r="C25">
+        <v>46000</v>
       </c>
       <c r="D25">
         <v>60.6</v>
@@ -1024,8 +898,8 @@
       <c r="B26" t="s">
         <v>27</v>
       </c>
-      <c r="C26" t="s">
-        <v>81</v>
+      <c r="C26">
+        <v>120000</v>
       </c>
       <c r="D26">
         <v>80.099999999999994</v>
@@ -1038,8 +912,8 @@
       <c r="B27" t="s">
         <v>28</v>
       </c>
-      <c r="C27" t="s">
-        <v>82</v>
+      <c r="C27">
+        <v>150000</v>
       </c>
       <c r="D27">
         <v>57.7</v>
@@ -1052,8 +926,8 @@
       <c r="B28" t="s">
         <v>29</v>
       </c>
-      <c r="C28" t="s">
-        <v>83</v>
+      <c r="C28">
+        <v>21000</v>
       </c>
       <c r="D28">
         <v>44.9</v>
@@ -1066,8 +940,8 @@
       <c r="B29" t="s">
         <v>30</v>
       </c>
-      <c r="C29" t="s">
-        <v>84</v>
+      <c r="C29">
+        <v>620000</v>
       </c>
       <c r="D29">
         <v>62.8</v>
@@ -1080,8 +954,8 @@
       <c r="B30" t="s">
         <v>31</v>
       </c>
-      <c r="C30" t="s">
-        <v>85</v>
+      <c r="C30">
+        <v>30000</v>
       </c>
       <c r="D30">
         <v>71</v>
@@ -1094,8 +968,8 @@
       <c r="B31" t="s">
         <v>32</v>
       </c>
-      <c r="C31" t="s">
-        <v>86</v>
+      <c r="C31">
+        <v>26000</v>
       </c>
       <c r="D31">
         <v>64.8</v>
@@ -1108,8 +982,8 @@
       <c r="B32" t="s">
         <v>33</v>
       </c>
-      <c r="C32" t="s">
-        <v>87</v>
+      <c r="C32">
+        <v>1600000</v>
       </c>
       <c r="D32">
         <v>11.9</v>
@@ -1136,8 +1010,8 @@
       <c r="B34" t="s">
         <v>35</v>
       </c>
-      <c r="C34" t="s">
-        <v>88</v>
+      <c r="C34">
+        <v>11000</v>
       </c>
       <c r="D34">
         <v>53.5</v>
@@ -1150,8 +1024,8 @@
       <c r="B35" t="s">
         <v>36</v>
       </c>
-      <c r="C35" t="s">
-        <v>89</v>
+      <c r="C35">
+        <v>330000</v>
       </c>
       <c r="D35">
         <v>13.9</v>
@@ -1164,8 +1038,8 @@
       <c r="B36" t="s">
         <v>37</v>
       </c>
-      <c r="C36" t="s">
-        <v>90</v>
+      <c r="C36">
+        <v>43000</v>
       </c>
       <c r="D36">
         <v>52.7</v>
@@ -1178,8 +1052,8 @@
       <c r="B37" t="s">
         <v>38</v>
       </c>
-      <c r="C37" t="s">
-        <v>91</v>
+      <c r="C37">
+        <v>1000000</v>
       </c>
       <c r="D37">
         <v>14.9</v>
@@ -1192,8 +1066,8 @@
       <c r="B38" t="s">
         <v>39</v>
       </c>
-      <c r="C38" t="s">
-        <v>92</v>
+      <c r="C38">
+        <v>110000</v>
       </c>
       <c r="D38">
         <v>45.8</v>
@@ -1207,7 +1081,7 @@
         <v>40</v>
       </c>
       <c r="C39" t="s">
-        <v>93</v>
+        <v>63</v>
       </c>
       <c r="D39">
         <v>75.599999999999994</v>
@@ -1221,7 +1095,7 @@
         <v>41</v>
       </c>
       <c r="C40" t="s">
-        <v>93</v>
+        <v>63</v>
       </c>
       <c r="D40">
         <v>52</v>
@@ -1234,8 +1108,8 @@
       <c r="B41" t="s">
         <v>42</v>
       </c>
-      <c r="C41" t="s">
-        <v>94</v>
+      <c r="C41">
+        <v>1800000</v>
       </c>
       <c r="D41">
         <v>28</v>
@@ -1248,8 +1122,8 @@
       <c r="B42" t="s">
         <v>43</v>
       </c>
-      <c r="C42" t="s">
-        <v>95</v>
+      <c r="C42">
+        <v>230000</v>
       </c>
       <c r="D42">
         <v>13</v>
@@ -1262,8 +1136,8 @@
       <c r="B43" t="s">
         <v>44</v>
       </c>
-      <c r="C43" t="s">
-        <v>96</v>
+      <c r="C43">
+        <v>32000</v>
       </c>
       <c r="D43">
         <v>28.3</v>
@@ -1276,8 +1150,8 @@
       <c r="B44" t="s">
         <v>45</v>
       </c>
-      <c r="C44" t="s">
-        <v>77</v>
+      <c r="C44">
+        <v>48000</v>
       </c>
       <c r="D44">
         <v>71.5</v>
@@ -1290,8 +1164,8 @@
       <c r="B45" t="s">
         <v>46</v>
       </c>
-      <c r="C45" t="s">
-        <v>97</v>
+      <c r="C45">
+        <v>3200000</v>
       </c>
       <c r="D45">
         <v>46.8</v>
@@ -1304,8 +1178,8 @@
       <c r="B46" t="s">
         <v>47</v>
       </c>
-      <c r="C46" t="s">
-        <v>70</v>
+      <c r="C46">
+        <v>130000</v>
       </c>
       <c r="D46">
         <v>49</v>
@@ -1318,8 +1192,8 @@
       <c r="B47" t="s">
         <v>48</v>
       </c>
-      <c r="C47" t="s">
-        <v>98</v>
+      <c r="C47">
+        <v>15000</v>
       </c>
       <c r="D47">
         <v>70.8</v>
@@ -1332,8 +1206,8 @@
       <c r="B48" t="s">
         <v>49</v>
       </c>
-      <c r="C48" t="s">
-        <v>99</v>
+      <c r="C48">
+        <v>220000</v>
       </c>
       <c r="D48">
         <v>9.9</v>
@@ -1360,8 +1234,8 @@
       <c r="B50" t="s">
         <v>51</v>
       </c>
-      <c r="C50" t="s">
-        <v>100</v>
+      <c r="C50">
+        <v>41000</v>
       </c>
       <c r="D50">
         <v>51.7</v>
@@ -1374,8 +1248,8 @@
       <c r="B51" t="s">
         <v>52</v>
       </c>
-      <c r="C51" t="s">
-        <v>63</v>
+      <c r="C51">
+        <v>67000</v>
       </c>
       <c r="D51">
         <v>53.4</v>
@@ -1388,8 +1262,8 @@
       <c r="B52" t="s">
         <v>53</v>
       </c>
-      <c r="C52" t="s">
-        <v>99</v>
+      <c r="C52">
+        <v>220000</v>
       </c>
       <c r="D52">
         <v>12.5</v>
@@ -1402,8 +1276,8 @@
       <c r="B53" t="s">
         <v>54</v>
       </c>
-      <c r="C53" t="s">
-        <v>101</v>
+      <c r="C53">
+        <v>100000</v>
       </c>
       <c r="D53">
         <v>45.8</v>
@@ -1416,8 +1290,8 @@
       <c r="B54" t="s">
         <v>55</v>
       </c>
-      <c r="C54" t="s">
-        <v>102</v>
+      <c r="C54">
+        <v>1400000</v>
       </c>
       <c r="D54">
         <v>26.2</v>
@@ -1430,8 +1304,8 @@
       <c r="B55" t="s">
         <v>56</v>
       </c>
-      <c r="C55" t="s">
-        <v>103</v>
+      <c r="C55">
+        <v>240000</v>
       </c>
       <c r="D55">
         <v>65.099999999999994</v>
@@ -1444,8 +1318,8 @@
       <c r="B56" t="s">
         <v>57</v>
       </c>
-      <c r="C56" t="s">
-        <v>102</v>
+      <c r="C56">
+        <v>1400000</v>
       </c>
       <c r="D56">
         <v>26.8</v>
@@ -1458,8 +1332,8 @@
       <c r="B57" t="s">
         <v>58</v>
       </c>
-      <c r="C57" t="s">
-        <v>104</v>
+      <c r="C57">
+        <v>1200000</v>
       </c>
       <c r="D57">
         <v>18</v>
@@ -1472,8 +1346,8 @@
       <c r="B58" t="s">
         <v>59</v>
       </c>
-      <c r="C58" t="s">
-        <v>105</v>
+      <c r="C58">
+        <v>1300000</v>
       </c>
       <c r="D58">
         <v>17.8</v>

</xml_diff>